<commit_message>
fixbug not found credentials file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="189">
   <si>
     <t xml:space="preserve">STT</t>
   </si>
@@ -526,9 +526,6 @@
     <t xml:space="preserve">28/10/1993</t>
   </si>
   <si>
-    <t xml:space="preserve">Kevin</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lê Quốc Khánh</t>
   </si>
   <si>
@@ -587,6 +584,9 @@
   </si>
   <si>
     <t xml:space="preserve">Phạm Hữu Vĩnh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23/02/2000</t>
   </si>
 </sst>
 </file>
@@ -697,15 +697,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L1038"/>
+  <dimension ref="A1:L1037"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J29" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.72"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -743,7 +757,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
@@ -781,7 +795,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
@@ -819,7 +833,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
@@ -853,7 +867,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
@@ -881,7 +895,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
@@ -915,7 +929,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
@@ -943,7 +957,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
@@ -979,7 +993,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
@@ -1007,7 +1021,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
@@ -1043,7 +1057,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
@@ -1071,7 +1085,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
@@ -1107,7 +1121,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
@@ -1141,7 +1155,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
@@ -1167,7 +1181,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
@@ -1201,7 +1215,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
@@ -1237,7 +1251,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
@@ -1269,7 +1283,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
@@ -1301,7 +1315,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>18</v>
       </c>
@@ -1337,7 +1351,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
@@ -1363,7 +1377,7 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
@@ -1399,7 +1413,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>21</v>
       </c>
@@ -1433,7 +1447,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>22</v>
       </c>
@@ -1467,7 +1481,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>23</v>
       </c>
@@ -1501,7 +1515,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>24</v>
       </c>
@@ -1535,7 +1549,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>25</v>
       </c>
@@ -1571,7 +1585,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>26</v>
       </c>
@@ -1591,7 +1605,7 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <v>27</v>
       </c>
@@ -1627,7 +1641,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
         <v>28</v>
       </c>
@@ -1655,7 +1669,7 @@
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
     </row>
-    <row r="30" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
         <v>29</v>
       </c>
@@ -1681,7 +1695,7 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
         <v>30</v>
       </c>
@@ -1709,16 +1723,20 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C32" s="3"/>
+      <c r="C32" s="1" t="s">
+        <v>169</v>
+      </c>
       <c r="D32" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E32" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="E32" s="1" t="n">
+        <v>906438113</v>
+      </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -1727,23 +1745,23 @@
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="D33" s="3"/>
       <c r="E33" s="1" t="n">
-        <v>906438113</v>
-      </c>
-      <c r="F33" s="3"/>
+        <v>979542273</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>172</v>
+      </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
@@ -1751,22 +1769,22 @@
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="1" t="n">
-        <v>979542273</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>173</v>
+        <v>969919088</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
@@ -1775,22 +1793,24 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D35" s="3"/>
+        <v>177</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E35" s="1" t="n">
-        <v>969919088</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>176</v>
+        <v>934407648</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>178</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
@@ -1799,24 +1819,24 @@
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E36" s="1" t="n">
-        <v>934407648</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>179</v>
+        <v>358483007</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -1825,24 +1845,24 @@
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>14</v>
+        <v>184</v>
       </c>
       <c r="E37" s="1" t="n">
-        <v>358483007</v>
+        <v>931996841</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
@@ -1851,18 +1871,18 @@
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="E38" s="1" t="n">
         <v>931996841</v>
@@ -1877,24 +1897,24 @@
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
     </row>
-    <row r="39" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="E39" s="1" t="n">
         <v>931996841</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
@@ -1903,31 +1923,18 @@
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="E40" s="1" t="n">
-        <v>931996841</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>187</v>
-      </c>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3"/>
@@ -1938,7 +1945,6 @@
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
     </row>
@@ -1951,6 +1957,7 @@
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
     </row>
@@ -1963,7 +1970,6 @@
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
     </row>
@@ -1976,6 +1982,7 @@
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
     </row>
@@ -1988,7 +1995,6 @@
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
     </row>
@@ -2001,6 +2007,7 @@
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
     </row>
@@ -2026,7 +2033,6 @@
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
     </row>
@@ -2039,6 +2045,7 @@
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
     </row>
@@ -2102,7 +2109,6 @@
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
@@ -2115,6 +2121,7 @@
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
@@ -2154,7 +2161,6 @@
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
-      <c r="I58" s="3"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
     </row>
@@ -2167,6 +2173,7 @@
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
     </row>
@@ -2192,7 +2199,6 @@
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
-      <c r="I61" s="3"/>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
     </row>
@@ -2205,6 +2211,7 @@
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
+      <c r="I62" s="3"/>
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
     </row>
@@ -2399,7 +2406,6 @@
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
-      <c r="I77" s="3"/>
       <c r="J77" s="3"/>
       <c r="K77" s="3"/>
     </row>
@@ -2424,6 +2430,7 @@
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
+      <c r="I79" s="3"/>
       <c r="J79" s="3"/>
       <c r="K79" s="3"/>
     </row>
@@ -2501,7 +2508,6 @@
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
-      <c r="I85" s="3"/>
       <c r="J85" s="3"/>
       <c r="K85" s="3"/>
     </row>
@@ -2514,6 +2520,7 @@
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
+      <c r="I86" s="3"/>
       <c r="J86" s="3"/>
       <c r="K86" s="3"/>
     </row>
@@ -2539,7 +2546,6 @@
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
-      <c r="I88" s="3"/>
       <c r="J88" s="3"/>
       <c r="K88" s="3"/>
     </row>
@@ -2552,6 +2558,7 @@
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
+      <c r="I89" s="3"/>
       <c r="J89" s="3"/>
       <c r="K89" s="3"/>
     </row>
@@ -2564,7 +2571,6 @@
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
-      <c r="I90" s="3"/>
       <c r="J90" s="3"/>
       <c r="K90" s="3"/>
     </row>
@@ -2577,6 +2583,7 @@
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
+      <c r="I91" s="3"/>
       <c r="J91" s="3"/>
       <c r="K91" s="3"/>
     </row>
@@ -2602,7 +2609,6 @@
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
-      <c r="I93" s="3"/>
       <c r="J93" s="3"/>
       <c r="K93" s="3"/>
     </row>
@@ -2615,6 +2621,7 @@
       <c r="F94" s="3"/>
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
+      <c r="I94" s="3"/>
       <c r="J94" s="3"/>
       <c r="K94" s="3"/>
     </row>
@@ -2770,7 +2777,6 @@
       <c r="F106" s="3"/>
       <c r="G106" s="3"/>
       <c r="H106" s="3"/>
-      <c r="I106" s="3"/>
       <c r="J106" s="3"/>
       <c r="K106" s="3"/>
     </row>
@@ -2783,6 +2789,7 @@
       <c r="F107" s="3"/>
       <c r="G107" s="3"/>
       <c r="H107" s="3"/>
+      <c r="I107" s="3"/>
       <c r="J107" s="3"/>
       <c r="K107" s="3"/>
     </row>
@@ -2808,7 +2815,6 @@
       <c r="F109" s="3"/>
       <c r="G109" s="3"/>
       <c r="H109" s="3"/>
-      <c r="I109" s="3"/>
       <c r="J109" s="3"/>
       <c r="K109" s="3"/>
     </row>
@@ -2833,6 +2839,7 @@
       <c r="F111" s="3"/>
       <c r="G111" s="3"/>
       <c r="H111" s="3"/>
+      <c r="I111" s="3"/>
       <c r="J111" s="3"/>
       <c r="K111" s="3"/>
     </row>
@@ -2884,7 +2891,6 @@
       <c r="F115" s="3"/>
       <c r="G115" s="3"/>
       <c r="H115" s="3"/>
-      <c r="I115" s="3"/>
       <c r="J115" s="3"/>
       <c r="K115" s="3"/>
     </row>
@@ -2909,6 +2915,7 @@
       <c r="F117" s="3"/>
       <c r="G117" s="3"/>
       <c r="H117" s="3"/>
+      <c r="I117" s="3"/>
       <c r="J117" s="3"/>
       <c r="K117" s="3"/>
     </row>
@@ -2934,7 +2941,6 @@
       <c r="F119" s="3"/>
       <c r="G119" s="3"/>
       <c r="H119" s="3"/>
-      <c r="I119" s="3"/>
       <c r="J119" s="3"/>
       <c r="K119" s="3"/>
     </row>
@@ -2947,6 +2953,7 @@
       <c r="F120" s="3"/>
       <c r="G120" s="3"/>
       <c r="H120" s="3"/>
+      <c r="I120" s="3"/>
       <c r="J120" s="3"/>
       <c r="K120" s="3"/>
     </row>
@@ -3011,7 +3018,6 @@
       <c r="F125" s="3"/>
       <c r="G125" s="3"/>
       <c r="H125" s="3"/>
-      <c r="I125" s="3"/>
       <c r="J125" s="3"/>
       <c r="K125" s="3"/>
     </row>
@@ -3024,6 +3030,7 @@
       <c r="F126" s="3"/>
       <c r="G126" s="3"/>
       <c r="H126" s="3"/>
+      <c r="I126" s="3"/>
       <c r="J126" s="3"/>
       <c r="K126" s="3"/>
     </row>
@@ -3101,7 +3108,6 @@
       <c r="F132" s="3"/>
       <c r="G132" s="3"/>
       <c r="H132" s="3"/>
-      <c r="I132" s="3"/>
       <c r="J132" s="3"/>
       <c r="K132" s="3"/>
     </row>
@@ -3114,6 +3120,7 @@
       <c r="F133" s="3"/>
       <c r="G133" s="3"/>
       <c r="H133" s="3"/>
+      <c r="I133" s="3"/>
       <c r="J133" s="3"/>
       <c r="K133" s="3"/>
     </row>
@@ -3139,7 +3146,6 @@
       <c r="F135" s="3"/>
       <c r="G135" s="3"/>
       <c r="H135" s="3"/>
-      <c r="I135" s="3"/>
       <c r="J135" s="3"/>
       <c r="K135" s="3"/>
     </row>
@@ -3152,6 +3158,7 @@
       <c r="F136" s="3"/>
       <c r="G136" s="3"/>
       <c r="H136" s="3"/>
+      <c r="I136" s="3"/>
       <c r="J136" s="3"/>
       <c r="K136" s="3"/>
     </row>
@@ -3216,7 +3223,6 @@
       <c r="F141" s="3"/>
       <c r="G141" s="3"/>
       <c r="H141" s="3"/>
-      <c r="I141" s="3"/>
       <c r="J141" s="3"/>
       <c r="K141" s="3"/>
     </row>
@@ -3229,6 +3235,7 @@
       <c r="F142" s="3"/>
       <c r="G142" s="3"/>
       <c r="H142" s="3"/>
+      <c r="I142" s="3"/>
       <c r="J142" s="3"/>
       <c r="K142" s="3"/>
     </row>
@@ -3293,7 +3300,6 @@
       <c r="F147" s="3"/>
       <c r="G147" s="3"/>
       <c r="H147" s="3"/>
-      <c r="I147" s="3"/>
       <c r="J147" s="3"/>
       <c r="K147" s="3"/>
     </row>
@@ -3306,6 +3312,7 @@
       <c r="F148" s="3"/>
       <c r="G148" s="3"/>
       <c r="H148" s="3"/>
+      <c r="I148" s="3"/>
       <c r="J148" s="3"/>
       <c r="K148" s="3"/>
     </row>
@@ -3383,7 +3390,6 @@
       <c r="F154" s="3"/>
       <c r="G154" s="3"/>
       <c r="H154" s="3"/>
-      <c r="I154" s="3"/>
       <c r="J154" s="3"/>
       <c r="K154" s="3"/>
     </row>
@@ -3396,6 +3402,7 @@
       <c r="F155" s="3"/>
       <c r="G155" s="3"/>
       <c r="H155" s="3"/>
+      <c r="I155" s="3"/>
       <c r="J155" s="3"/>
       <c r="K155" s="3"/>
     </row>
@@ -3512,7 +3519,6 @@
       <c r="F164" s="3"/>
       <c r="G164" s="3"/>
       <c r="H164" s="3"/>
-      <c r="I164" s="3"/>
       <c r="J164" s="3"/>
       <c r="K164" s="3"/>
     </row>
@@ -3525,6 +3531,7 @@
       <c r="F165" s="3"/>
       <c r="G165" s="3"/>
       <c r="H165" s="3"/>
+      <c r="I165" s="3"/>
       <c r="J165" s="3"/>
       <c r="K165" s="3"/>
     </row>
@@ -3576,7 +3583,6 @@
       <c r="F169" s="3"/>
       <c r="G169" s="3"/>
       <c r="H169" s="3"/>
-      <c r="I169" s="3"/>
       <c r="J169" s="3"/>
       <c r="K169" s="3"/>
     </row>
@@ -3601,6 +3607,7 @@
       <c r="F171" s="3"/>
       <c r="G171" s="3"/>
       <c r="H171" s="3"/>
+      <c r="I171" s="3"/>
       <c r="J171" s="3"/>
       <c r="K171" s="3"/>
     </row>
@@ -3613,7 +3620,6 @@
       <c r="F172" s="3"/>
       <c r="G172" s="3"/>
       <c r="H172" s="3"/>
-      <c r="I172" s="3"/>
       <c r="J172" s="3"/>
       <c r="K172" s="3"/>
     </row>
@@ -3626,6 +3632,7 @@
       <c r="F173" s="3"/>
       <c r="G173" s="3"/>
       <c r="H173" s="3"/>
+      <c r="I173" s="3"/>
       <c r="J173" s="3"/>
       <c r="K173" s="3"/>
     </row>
@@ -3651,7 +3658,6 @@
       <c r="F175" s="3"/>
       <c r="G175" s="3"/>
       <c r="H175" s="3"/>
-      <c r="I175" s="3"/>
       <c r="J175" s="3"/>
       <c r="K175" s="3"/>
     </row>
@@ -3688,6 +3694,7 @@
       <c r="F178" s="3"/>
       <c r="G178" s="3"/>
       <c r="H178" s="3"/>
+      <c r="I178" s="3"/>
       <c r="J178" s="3"/>
       <c r="K178" s="3"/>
     </row>
@@ -3817,7 +3824,6 @@
       <c r="F188" s="3"/>
       <c r="G188" s="3"/>
       <c r="H188" s="3"/>
-      <c r="I188" s="3"/>
       <c r="J188" s="3"/>
       <c r="K188" s="3"/>
     </row>
@@ -3830,6 +3836,7 @@
       <c r="F189" s="3"/>
       <c r="G189" s="3"/>
       <c r="H189" s="3"/>
+      <c r="I189" s="3"/>
       <c r="J189" s="3"/>
       <c r="K189" s="3"/>
     </row>
@@ -3894,7 +3901,6 @@
       <c r="F194" s="3"/>
       <c r="G194" s="3"/>
       <c r="H194" s="3"/>
-      <c r="I194" s="3"/>
       <c r="J194" s="3"/>
       <c r="K194" s="3"/>
     </row>
@@ -3907,6 +3913,7 @@
       <c r="F195" s="3"/>
       <c r="G195" s="3"/>
       <c r="H195" s="3"/>
+      <c r="I195" s="3"/>
       <c r="J195" s="3"/>
       <c r="K195" s="3"/>
     </row>
@@ -3932,7 +3939,6 @@
       <c r="F197" s="3"/>
       <c r="G197" s="3"/>
       <c r="H197" s="3"/>
-      <c r="I197" s="3"/>
       <c r="J197" s="3"/>
       <c r="K197" s="3"/>
     </row>
@@ -3945,6 +3951,7 @@
       <c r="F198" s="3"/>
       <c r="G198" s="3"/>
       <c r="H198" s="3"/>
+      <c r="I198" s="3"/>
       <c r="J198" s="3"/>
       <c r="K198" s="3"/>
     </row>
@@ -3957,7 +3964,6 @@
       <c r="F199" s="3"/>
       <c r="G199" s="3"/>
       <c r="H199" s="3"/>
-      <c r="I199" s="3"/>
       <c r="J199" s="3"/>
       <c r="K199" s="3"/>
     </row>
@@ -3970,6 +3976,7 @@
       <c r="F200" s="3"/>
       <c r="G200" s="3"/>
       <c r="H200" s="3"/>
+      <c r="I200" s="3"/>
       <c r="J200" s="3"/>
       <c r="K200" s="3"/>
     </row>
@@ -3982,7 +3989,6 @@
       <c r="F201" s="3"/>
       <c r="G201" s="3"/>
       <c r="H201" s="3"/>
-      <c r="I201" s="3"/>
       <c r="J201" s="3"/>
       <c r="K201" s="3"/>
     </row>
@@ -4031,6 +4037,7 @@
       <c r="F205" s="3"/>
       <c r="G205" s="3"/>
       <c r="H205" s="3"/>
+      <c r="I205" s="3"/>
       <c r="J205" s="3"/>
       <c r="K205" s="3"/>
     </row>
@@ -4069,7 +4076,6 @@
       <c r="F208" s="3"/>
       <c r="G208" s="3"/>
       <c r="H208" s="3"/>
-      <c r="I208" s="3"/>
       <c r="J208" s="3"/>
       <c r="K208" s="3"/>
     </row>
@@ -4082,6 +4088,7 @@
       <c r="F209" s="3"/>
       <c r="G209" s="3"/>
       <c r="H209" s="3"/>
+      <c r="I209" s="3"/>
       <c r="J209" s="3"/>
       <c r="K209" s="3"/>
     </row>
@@ -4107,7 +4114,6 @@
       <c r="F211" s="3"/>
       <c r="G211" s="3"/>
       <c r="H211" s="3"/>
-      <c r="I211" s="3"/>
       <c r="J211" s="3"/>
       <c r="K211" s="3"/>
     </row>
@@ -4120,6 +4126,7 @@
       <c r="F212" s="3"/>
       <c r="G212" s="3"/>
       <c r="H212" s="3"/>
+      <c r="I212" s="3"/>
       <c r="J212" s="3"/>
       <c r="K212" s="3"/>
     </row>
@@ -4132,7 +4139,6 @@
       <c r="F213" s="3"/>
       <c r="G213" s="3"/>
       <c r="H213" s="3"/>
-      <c r="I213" s="3"/>
       <c r="J213" s="3"/>
       <c r="K213" s="3"/>
     </row>
@@ -4145,6 +4151,7 @@
       <c r="F214" s="3"/>
       <c r="G214" s="3"/>
       <c r="H214" s="3"/>
+      <c r="I214" s="3"/>
       <c r="J214" s="3"/>
       <c r="K214" s="3"/>
     </row>
@@ -4170,7 +4177,6 @@
       <c r="F216" s="3"/>
       <c r="G216" s="3"/>
       <c r="H216" s="3"/>
-      <c r="I216" s="3"/>
       <c r="J216" s="3"/>
       <c r="K216" s="3"/>
     </row>
@@ -4183,6 +4189,7 @@
       <c r="F217" s="3"/>
       <c r="G217" s="3"/>
       <c r="H217" s="3"/>
+      <c r="I217" s="3"/>
       <c r="J217" s="3"/>
       <c r="K217" s="3"/>
     </row>
@@ -4208,7 +4215,6 @@
       <c r="F219" s="3"/>
       <c r="G219" s="3"/>
       <c r="H219" s="3"/>
-      <c r="I219" s="3"/>
       <c r="J219" s="3"/>
       <c r="K219" s="3"/>
     </row>
@@ -4233,6 +4239,7 @@
       <c r="F221" s="3"/>
       <c r="G221" s="3"/>
       <c r="H221" s="3"/>
+      <c r="I221" s="3"/>
       <c r="J221" s="3"/>
       <c r="K221" s="3"/>
     </row>
@@ -4271,7 +4278,6 @@
       <c r="F224" s="3"/>
       <c r="G224" s="3"/>
       <c r="H224" s="3"/>
-      <c r="I224" s="3"/>
       <c r="J224" s="3"/>
       <c r="K224" s="3"/>
     </row>
@@ -4284,6 +4290,7 @@
       <c r="F225" s="3"/>
       <c r="G225" s="3"/>
       <c r="H225" s="3"/>
+      <c r="I225" s="3"/>
       <c r="J225" s="3"/>
       <c r="K225" s="3"/>
     </row>
@@ -4387,7 +4394,6 @@
       <c r="F233" s="3"/>
       <c r="G233" s="3"/>
       <c r="H233" s="3"/>
-      <c r="I233" s="3"/>
       <c r="J233" s="3"/>
       <c r="K233" s="3"/>
     </row>
@@ -4400,6 +4406,7 @@
       <c r="F234" s="3"/>
       <c r="G234" s="3"/>
       <c r="H234" s="3"/>
+      <c r="I234" s="3"/>
       <c r="J234" s="3"/>
       <c r="K234" s="3"/>
     </row>
@@ -4438,7 +4445,6 @@
       <c r="F237" s="3"/>
       <c r="G237" s="3"/>
       <c r="H237" s="3"/>
-      <c r="I237" s="3"/>
       <c r="J237" s="3"/>
       <c r="K237" s="3"/>
     </row>
@@ -4463,6 +4469,7 @@
       <c r="F239" s="3"/>
       <c r="G239" s="3"/>
       <c r="H239" s="3"/>
+      <c r="I239" s="3"/>
       <c r="J239" s="3"/>
       <c r="K239" s="3"/>
     </row>
@@ -4488,7 +4495,6 @@
       <c r="F241" s="3"/>
       <c r="G241" s="3"/>
       <c r="H241" s="3"/>
-      <c r="I241" s="3"/>
       <c r="J241" s="3"/>
       <c r="K241" s="3"/>
     </row>
@@ -4501,6 +4507,7 @@
       <c r="F242" s="3"/>
       <c r="G242" s="3"/>
       <c r="H242" s="3"/>
+      <c r="I242" s="3"/>
       <c r="J242" s="3"/>
       <c r="K242" s="3"/>
     </row>
@@ -4513,7 +4520,6 @@
       <c r="F243" s="3"/>
       <c r="G243" s="3"/>
       <c r="H243" s="3"/>
-      <c r="I243" s="3"/>
       <c r="J243" s="3"/>
       <c r="K243" s="3"/>
     </row>
@@ -4526,6 +4532,7 @@
       <c r="F244" s="3"/>
       <c r="G244" s="3"/>
       <c r="H244" s="3"/>
+      <c r="I244" s="3"/>
       <c r="J244" s="3"/>
       <c r="K244" s="3"/>
     </row>
@@ -4577,7 +4584,6 @@
       <c r="F248" s="3"/>
       <c r="G248" s="3"/>
       <c r="H248" s="3"/>
-      <c r="I248" s="3"/>
       <c r="J248" s="3"/>
       <c r="K248" s="3"/>
     </row>
@@ -4590,6 +4596,7 @@
       <c r="F249" s="3"/>
       <c r="G249" s="3"/>
       <c r="H249" s="3"/>
+      <c r="I249" s="3"/>
       <c r="J249" s="3"/>
       <c r="K249" s="3"/>
     </row>
@@ -4615,7 +4622,6 @@
       <c r="F251" s="3"/>
       <c r="G251" s="3"/>
       <c r="H251" s="3"/>
-      <c r="I251" s="3"/>
       <c r="J251" s="3"/>
       <c r="K251" s="3"/>
     </row>
@@ -4664,6 +4670,7 @@
       <c r="F255" s="3"/>
       <c r="G255" s="3"/>
       <c r="H255" s="3"/>
+      <c r="I255" s="3"/>
       <c r="J255" s="3"/>
       <c r="K255" s="3"/>
     </row>
@@ -4728,7 +4735,6 @@
       <c r="F260" s="3"/>
       <c r="G260" s="3"/>
       <c r="H260" s="3"/>
-      <c r="I260" s="3"/>
       <c r="J260" s="3"/>
       <c r="K260" s="3"/>
     </row>
@@ -4753,6 +4759,7 @@
       <c r="F262" s="3"/>
       <c r="G262" s="3"/>
       <c r="H262" s="3"/>
+      <c r="I262" s="3"/>
       <c r="J262" s="3"/>
       <c r="K262" s="3"/>
     </row>
@@ -4765,7 +4772,6 @@
       <c r="F263" s="3"/>
       <c r="G263" s="3"/>
       <c r="H263" s="3"/>
-      <c r="I263" s="3"/>
       <c r="J263" s="3"/>
       <c r="K263" s="3"/>
     </row>
@@ -4778,6 +4784,7 @@
       <c r="F264" s="3"/>
       <c r="G264" s="3"/>
       <c r="H264" s="3"/>
+      <c r="I264" s="3"/>
       <c r="J264" s="3"/>
       <c r="K264" s="3"/>
     </row>
@@ -4816,7 +4823,6 @@
       <c r="F267" s="3"/>
       <c r="G267" s="3"/>
       <c r="H267" s="3"/>
-      <c r="I267" s="3"/>
       <c r="J267" s="3"/>
       <c r="K267" s="3"/>
     </row>
@@ -4841,6 +4847,7 @@
       <c r="F269" s="3"/>
       <c r="G269" s="3"/>
       <c r="H269" s="3"/>
+      <c r="I269" s="3"/>
       <c r="J269" s="3"/>
       <c r="K269" s="3"/>
     </row>
@@ -4853,7 +4860,6 @@
       <c r="F270" s="3"/>
       <c r="G270" s="3"/>
       <c r="H270" s="3"/>
-      <c r="I270" s="3"/>
       <c r="J270" s="3"/>
       <c r="K270" s="3"/>
     </row>
@@ -4866,6 +4872,7 @@
       <c r="F271" s="3"/>
       <c r="G271" s="3"/>
       <c r="H271" s="3"/>
+      <c r="I271" s="3"/>
       <c r="J271" s="3"/>
       <c r="K271" s="3"/>
     </row>
@@ -4878,7 +4885,6 @@
       <c r="F272" s="3"/>
       <c r="G272" s="3"/>
       <c r="H272" s="3"/>
-      <c r="I272" s="3"/>
       <c r="J272" s="3"/>
       <c r="K272" s="3"/>
     </row>
@@ -4891,6 +4897,7 @@
       <c r="F273" s="3"/>
       <c r="G273" s="3"/>
       <c r="H273" s="3"/>
+      <c r="I273" s="3"/>
       <c r="J273" s="3"/>
       <c r="K273" s="3"/>
     </row>
@@ -4903,7 +4910,6 @@
       <c r="F274" s="3"/>
       <c r="G274" s="3"/>
       <c r="H274" s="3"/>
-      <c r="I274" s="3"/>
       <c r="J274" s="3"/>
       <c r="K274" s="3"/>
     </row>
@@ -4940,6 +4946,7 @@
       <c r="F277" s="3"/>
       <c r="G277" s="3"/>
       <c r="H277" s="3"/>
+      <c r="I277" s="3"/>
       <c r="J277" s="3"/>
       <c r="K277" s="3"/>
     </row>
@@ -4952,7 +4959,6 @@
       <c r="F278" s="3"/>
       <c r="G278" s="3"/>
       <c r="H278" s="3"/>
-      <c r="I278" s="3"/>
       <c r="J278" s="3"/>
       <c r="K278" s="3"/>
     </row>
@@ -4965,6 +4971,7 @@
       <c r="F279" s="3"/>
       <c r="G279" s="3"/>
       <c r="H279" s="3"/>
+      <c r="I279" s="3"/>
       <c r="J279" s="3"/>
       <c r="K279" s="3"/>
     </row>
@@ -4990,7 +4997,6 @@
       <c r="F281" s="3"/>
       <c r="G281" s="3"/>
       <c r="H281" s="3"/>
-      <c r="I281" s="3"/>
       <c r="J281" s="3"/>
       <c r="K281" s="3"/>
     </row>
@@ -5003,6 +5009,7 @@
       <c r="F282" s="3"/>
       <c r="G282" s="3"/>
       <c r="H282" s="3"/>
+      <c r="I282" s="3"/>
       <c r="J282" s="3"/>
       <c r="K282" s="3"/>
     </row>
@@ -5028,7 +5035,6 @@
       <c r="F284" s="3"/>
       <c r="G284" s="3"/>
       <c r="H284" s="3"/>
-      <c r="I284" s="3"/>
       <c r="J284" s="3"/>
       <c r="K284" s="3"/>
     </row>
@@ -5041,6 +5047,7 @@
       <c r="F285" s="3"/>
       <c r="G285" s="3"/>
       <c r="H285" s="3"/>
+      <c r="I285" s="3"/>
       <c r="J285" s="3"/>
       <c r="K285" s="3"/>
     </row>
@@ -5079,7 +5086,6 @@
       <c r="F288" s="3"/>
       <c r="G288" s="3"/>
       <c r="H288" s="3"/>
-      <c r="I288" s="3"/>
       <c r="J288" s="3"/>
       <c r="K288" s="3"/>
     </row>
@@ -5092,6 +5098,7 @@
       <c r="F289" s="3"/>
       <c r="G289" s="3"/>
       <c r="H289" s="3"/>
+      <c r="I289" s="3"/>
       <c r="J289" s="3"/>
       <c r="K289" s="3"/>
     </row>
@@ -5104,7 +5111,6 @@
       <c r="F290" s="3"/>
       <c r="G290" s="3"/>
       <c r="H290" s="3"/>
-      <c r="I290" s="3"/>
       <c r="J290" s="3"/>
       <c r="K290" s="3"/>
     </row>
@@ -5117,6 +5123,7 @@
       <c r="F291" s="3"/>
       <c r="G291" s="3"/>
       <c r="H291" s="3"/>
+      <c r="I291" s="3"/>
       <c r="J291" s="3"/>
       <c r="K291" s="3"/>
     </row>
@@ -5142,7 +5149,6 @@
       <c r="F293" s="3"/>
       <c r="G293" s="3"/>
       <c r="H293" s="3"/>
-      <c r="I293" s="3"/>
       <c r="J293" s="3"/>
       <c r="K293" s="3"/>
     </row>
@@ -5155,6 +5161,7 @@
       <c r="F294" s="3"/>
       <c r="G294" s="3"/>
       <c r="H294" s="3"/>
+      <c r="I294" s="3"/>
       <c r="J294" s="3"/>
       <c r="K294" s="3"/>
     </row>
@@ -5193,7 +5200,6 @@
       <c r="F297" s="3"/>
       <c r="G297" s="3"/>
       <c r="H297" s="3"/>
-      <c r="I297" s="3"/>
       <c r="J297" s="3"/>
       <c r="K297" s="3"/>
     </row>
@@ -5206,6 +5212,7 @@
       <c r="F298" s="3"/>
       <c r="G298" s="3"/>
       <c r="H298" s="3"/>
+      <c r="I298" s="3"/>
       <c r="J298" s="3"/>
       <c r="K298" s="3"/>
     </row>
@@ -5257,7 +5264,6 @@
       <c r="F302" s="3"/>
       <c r="G302" s="3"/>
       <c r="H302" s="3"/>
-      <c r="I302" s="3"/>
       <c r="J302" s="3"/>
       <c r="K302" s="3"/>
     </row>
@@ -5270,6 +5276,7 @@
       <c r="F303" s="3"/>
       <c r="G303" s="3"/>
       <c r="H303" s="3"/>
+      <c r="I303" s="3"/>
       <c r="J303" s="3"/>
       <c r="K303" s="3"/>
     </row>
@@ -5295,7 +5302,6 @@
       <c r="F305" s="3"/>
       <c r="G305" s="3"/>
       <c r="H305" s="3"/>
-      <c r="I305" s="3"/>
       <c r="J305" s="3"/>
       <c r="K305" s="3"/>
     </row>
@@ -5308,6 +5314,7 @@
       <c r="F306" s="3"/>
       <c r="G306" s="3"/>
       <c r="H306" s="3"/>
+      <c r="I306" s="3"/>
       <c r="J306" s="3"/>
       <c r="K306" s="3"/>
     </row>
@@ -5398,7 +5405,6 @@
       <c r="F313" s="3"/>
       <c r="G313" s="3"/>
       <c r="H313" s="3"/>
-      <c r="I313" s="3"/>
       <c r="J313" s="3"/>
       <c r="K313" s="3"/>
     </row>
@@ -5435,6 +5441,7 @@
       <c r="F316" s="3"/>
       <c r="G316" s="3"/>
       <c r="H316" s="3"/>
+      <c r="I316" s="3"/>
       <c r="J316" s="3"/>
       <c r="K316" s="3"/>
     </row>
@@ -5460,7 +5467,6 @@
       <c r="F318" s="3"/>
       <c r="G318" s="3"/>
       <c r="H318" s="3"/>
-      <c r="I318" s="3"/>
       <c r="J318" s="3"/>
       <c r="K318" s="3"/>
     </row>
@@ -5473,6 +5479,7 @@
       <c r="F319" s="3"/>
       <c r="G319" s="3"/>
       <c r="H319" s="3"/>
+      <c r="I319" s="3"/>
       <c r="J319" s="3"/>
       <c r="K319" s="3"/>
     </row>
@@ -5524,7 +5531,6 @@
       <c r="F323" s="3"/>
       <c r="G323" s="3"/>
       <c r="H323" s="3"/>
-      <c r="I323" s="3"/>
       <c r="J323" s="3"/>
       <c r="K323" s="3"/>
     </row>
@@ -5549,6 +5555,7 @@
       <c r="F325" s="3"/>
       <c r="G325" s="3"/>
       <c r="H325" s="3"/>
+      <c r="I325" s="3"/>
       <c r="J325" s="3"/>
       <c r="K325" s="3"/>
     </row>
@@ -5574,7 +5581,6 @@
       <c r="F327" s="3"/>
       <c r="G327" s="3"/>
       <c r="H327" s="3"/>
-      <c r="I327" s="3"/>
       <c r="J327" s="3"/>
       <c r="K327" s="3"/>
     </row>
@@ -5587,6 +5593,7 @@
       <c r="F328" s="3"/>
       <c r="G328" s="3"/>
       <c r="H328" s="3"/>
+      <c r="I328" s="3"/>
       <c r="J328" s="3"/>
       <c r="K328" s="3"/>
     </row>
@@ -5651,7 +5658,6 @@
       <c r="F333" s="3"/>
       <c r="G333" s="3"/>
       <c r="H333" s="3"/>
-      <c r="I333" s="3"/>
       <c r="J333" s="3"/>
       <c r="K333" s="3"/>
     </row>
@@ -5664,6 +5670,7 @@
       <c r="F334" s="3"/>
       <c r="G334" s="3"/>
       <c r="H334" s="3"/>
+      <c r="I334" s="3"/>
       <c r="J334" s="3"/>
       <c r="K334" s="3"/>
     </row>
@@ -5780,7 +5787,6 @@
       <c r="F343" s="3"/>
       <c r="G343" s="3"/>
       <c r="H343" s="3"/>
-      <c r="I343" s="3"/>
       <c r="J343" s="3"/>
       <c r="K343" s="3"/>
     </row>
@@ -5793,6 +5799,7 @@
       <c r="F344" s="3"/>
       <c r="G344" s="3"/>
       <c r="H344" s="3"/>
+      <c r="I344" s="3"/>
       <c r="J344" s="3"/>
       <c r="K344" s="3"/>
     </row>
@@ -5818,7 +5825,6 @@
       <c r="F346" s="3"/>
       <c r="G346" s="3"/>
       <c r="H346" s="3"/>
-      <c r="I346" s="3"/>
       <c r="J346" s="3"/>
       <c r="K346" s="3"/>
     </row>
@@ -5831,6 +5837,7 @@
       <c r="F347" s="3"/>
       <c r="G347" s="3"/>
       <c r="H347" s="3"/>
+      <c r="I347" s="3"/>
       <c r="J347" s="3"/>
       <c r="K347" s="3"/>
     </row>
@@ -5869,7 +5876,6 @@
       <c r="F350" s="3"/>
       <c r="G350" s="3"/>
       <c r="H350" s="3"/>
-      <c r="I350" s="3"/>
       <c r="J350" s="3"/>
       <c r="K350" s="3"/>
     </row>
@@ -5882,6 +5888,7 @@
       <c r="F351" s="3"/>
       <c r="G351" s="3"/>
       <c r="H351" s="3"/>
+      <c r="I351" s="3"/>
       <c r="J351" s="3"/>
       <c r="K351" s="3"/>
     </row>
@@ -5920,7 +5927,6 @@
       <c r="F354" s="3"/>
       <c r="G354" s="3"/>
       <c r="H354" s="3"/>
-      <c r="I354" s="3"/>
       <c r="J354" s="3"/>
       <c r="K354" s="3"/>
     </row>
@@ -5945,6 +5951,7 @@
       <c r="F356" s="3"/>
       <c r="G356" s="3"/>
       <c r="H356" s="3"/>
+      <c r="I356" s="3"/>
       <c r="J356" s="3"/>
       <c r="K356" s="3"/>
     </row>
@@ -5970,7 +5977,6 @@
       <c r="F358" s="3"/>
       <c r="G358" s="3"/>
       <c r="H358" s="3"/>
-      <c r="I358" s="3"/>
       <c r="J358" s="3"/>
       <c r="K358" s="3"/>
     </row>
@@ -5983,6 +5989,7 @@
       <c r="F359" s="3"/>
       <c r="G359" s="3"/>
       <c r="H359" s="3"/>
+      <c r="I359" s="3"/>
       <c r="J359" s="3"/>
       <c r="K359" s="3"/>
     </row>
@@ -6021,7 +6028,6 @@
       <c r="F362" s="3"/>
       <c r="G362" s="3"/>
       <c r="H362" s="3"/>
-      <c r="I362" s="3"/>
       <c r="J362" s="3"/>
       <c r="K362" s="3"/>
     </row>
@@ -6034,6 +6040,7 @@
       <c r="F363" s="3"/>
       <c r="G363" s="3"/>
       <c r="H363" s="3"/>
+      <c r="I363" s="3"/>
       <c r="J363" s="3"/>
       <c r="K363" s="3"/>
     </row>
@@ -6111,7 +6118,6 @@
       <c r="F369" s="3"/>
       <c r="G369" s="3"/>
       <c r="H369" s="3"/>
-      <c r="I369" s="3"/>
       <c r="J369" s="3"/>
       <c r="K369" s="3"/>
     </row>
@@ -6124,6 +6130,7 @@
       <c r="F370" s="3"/>
       <c r="G370" s="3"/>
       <c r="H370" s="3"/>
+      <c r="I370" s="3"/>
       <c r="J370" s="3"/>
       <c r="K370" s="3"/>
     </row>
@@ -6136,7 +6143,6 @@
       <c r="F371" s="3"/>
       <c r="G371" s="3"/>
       <c r="H371" s="3"/>
-      <c r="I371" s="3"/>
       <c r="J371" s="3"/>
       <c r="K371" s="3"/>
     </row>
@@ -6149,6 +6155,7 @@
       <c r="F372" s="3"/>
       <c r="G372" s="3"/>
       <c r="H372" s="3"/>
+      <c r="I372" s="3"/>
       <c r="J372" s="3"/>
       <c r="K372" s="3"/>
     </row>
@@ -6174,7 +6181,6 @@
       <c r="F374" s="3"/>
       <c r="G374" s="3"/>
       <c r="H374" s="3"/>
-      <c r="I374" s="3"/>
       <c r="J374" s="3"/>
       <c r="K374" s="3"/>
     </row>
@@ -6187,6 +6193,7 @@
       <c r="F375" s="3"/>
       <c r="G375" s="3"/>
       <c r="H375" s="3"/>
+      <c r="I375" s="3"/>
       <c r="J375" s="3"/>
       <c r="K375" s="3"/>
     </row>
@@ -6264,7 +6271,6 @@
       <c r="F381" s="3"/>
       <c r="G381" s="3"/>
       <c r="H381" s="3"/>
-      <c r="I381" s="3"/>
       <c r="J381" s="3"/>
       <c r="K381" s="3"/>
     </row>
@@ -6277,6 +6283,7 @@
       <c r="F382" s="3"/>
       <c r="G382" s="3"/>
       <c r="H382" s="3"/>
+      <c r="I382" s="3"/>
       <c r="J382" s="3"/>
       <c r="K382" s="3"/>
     </row>
@@ -6302,7 +6309,6 @@
       <c r="F384" s="3"/>
       <c r="G384" s="3"/>
       <c r="H384" s="3"/>
-      <c r="I384" s="3"/>
       <c r="J384" s="3"/>
       <c r="K384" s="3"/>
     </row>
@@ -6327,6 +6333,7 @@
       <c r="F386" s="3"/>
       <c r="G386" s="3"/>
       <c r="H386" s="3"/>
+      <c r="I386" s="3"/>
       <c r="J386" s="3"/>
       <c r="K386" s="3"/>
     </row>
@@ -6391,7 +6398,6 @@
       <c r="F391" s="3"/>
       <c r="G391" s="3"/>
       <c r="H391" s="3"/>
-      <c r="I391" s="3"/>
       <c r="J391" s="3"/>
       <c r="K391" s="3"/>
     </row>
@@ -6404,6 +6410,7 @@
       <c r="F392" s="3"/>
       <c r="G392" s="3"/>
       <c r="H392" s="3"/>
+      <c r="I392" s="3"/>
       <c r="J392" s="3"/>
       <c r="K392" s="3"/>
     </row>
@@ -6416,7 +6423,6 @@
       <c r="F393" s="3"/>
       <c r="G393" s="3"/>
       <c r="H393" s="3"/>
-      <c r="I393" s="3"/>
       <c r="J393" s="3"/>
       <c r="K393" s="3"/>
     </row>
@@ -6429,6 +6435,7 @@
       <c r="F394" s="3"/>
       <c r="G394" s="3"/>
       <c r="H394" s="3"/>
+      <c r="I394" s="3"/>
       <c r="J394" s="3"/>
       <c r="K394" s="3"/>
     </row>
@@ -6441,7 +6448,6 @@
       <c r="F395" s="3"/>
       <c r="G395" s="3"/>
       <c r="H395" s="3"/>
-      <c r="I395" s="3"/>
       <c r="J395" s="3"/>
       <c r="K395" s="3"/>
     </row>
@@ -6478,6 +6484,7 @@
       <c r="F398" s="3"/>
       <c r="G398" s="3"/>
       <c r="H398" s="3"/>
+      <c r="I398" s="3"/>
       <c r="J398" s="3"/>
       <c r="K398" s="3"/>
     </row>
@@ -6503,7 +6510,6 @@
       <c r="F400" s="3"/>
       <c r="G400" s="3"/>
       <c r="H400" s="3"/>
-      <c r="I400" s="3"/>
       <c r="J400" s="3"/>
       <c r="K400" s="3"/>
     </row>
@@ -6516,6 +6522,7 @@
       <c r="F401" s="3"/>
       <c r="G401" s="3"/>
       <c r="H401" s="3"/>
+      <c r="I401" s="3"/>
       <c r="J401" s="3"/>
       <c r="K401" s="3"/>
     </row>
@@ -6528,7 +6535,6 @@
       <c r="F402" s="3"/>
       <c r="G402" s="3"/>
       <c r="H402" s="3"/>
-      <c r="I402" s="3"/>
       <c r="J402" s="3"/>
       <c r="K402" s="3"/>
     </row>
@@ -6541,6 +6547,7 @@
       <c r="F403" s="3"/>
       <c r="G403" s="3"/>
       <c r="H403" s="3"/>
+      <c r="I403" s="3"/>
       <c r="J403" s="3"/>
       <c r="K403" s="3"/>
     </row>
@@ -6553,7 +6560,6 @@
       <c r="F404" s="3"/>
       <c r="G404" s="3"/>
       <c r="H404" s="3"/>
-      <c r="I404" s="3"/>
       <c r="J404" s="3"/>
       <c r="K404" s="3"/>
     </row>
@@ -6566,6 +6572,7 @@
       <c r="F405" s="3"/>
       <c r="G405" s="3"/>
       <c r="H405" s="3"/>
+      <c r="I405" s="3"/>
       <c r="J405" s="3"/>
       <c r="K405" s="3"/>
     </row>
@@ -6656,7 +6663,6 @@
       <c r="F412" s="3"/>
       <c r="G412" s="3"/>
       <c r="H412" s="3"/>
-      <c r="I412" s="3"/>
       <c r="J412" s="3"/>
       <c r="K412" s="3"/>
     </row>
@@ -6681,6 +6687,7 @@
       <c r="F414" s="3"/>
       <c r="G414" s="3"/>
       <c r="H414" s="3"/>
+      <c r="I414" s="3"/>
       <c r="J414" s="3"/>
       <c r="K414" s="3"/>
     </row>
@@ -6758,7 +6765,6 @@
       <c r="F420" s="3"/>
       <c r="G420" s="3"/>
       <c r="H420" s="3"/>
-      <c r="I420" s="3"/>
       <c r="J420" s="3"/>
       <c r="K420" s="3"/>
     </row>
@@ -6771,6 +6777,7 @@
       <c r="F421" s="3"/>
       <c r="G421" s="3"/>
       <c r="H421" s="3"/>
+      <c r="I421" s="3"/>
       <c r="J421" s="3"/>
       <c r="K421" s="3"/>
     </row>
@@ -6796,7 +6803,6 @@
       <c r="F423" s="3"/>
       <c r="G423" s="3"/>
       <c r="H423" s="3"/>
-      <c r="I423" s="3"/>
       <c r="J423" s="3"/>
       <c r="K423" s="3"/>
     </row>
@@ -6820,7 +6826,7 @@
       <c r="E425" s="3"/>
       <c r="F425" s="3"/>
       <c r="G425" s="3"/>
-      <c r="H425" s="3"/>
+      <c r="I425" s="3"/>
       <c r="J425" s="3"/>
       <c r="K425" s="3"/>
     </row>
@@ -6832,6 +6838,7 @@
       <c r="E426" s="3"/>
       <c r="F426" s="3"/>
       <c r="G426" s="3"/>
+      <c r="H426" s="3"/>
       <c r="I426" s="3"/>
       <c r="J426" s="3"/>
       <c r="K426" s="3"/>
@@ -6910,7 +6917,6 @@
       <c r="F432" s="3"/>
       <c r="G432" s="3"/>
       <c r="H432" s="3"/>
-      <c r="I432" s="3"/>
       <c r="J432" s="3"/>
       <c r="K432" s="3"/>
     </row>
@@ -6947,6 +6953,7 @@
       <c r="F435" s="3"/>
       <c r="G435" s="3"/>
       <c r="H435" s="3"/>
+      <c r="I435" s="3"/>
       <c r="J435" s="3"/>
       <c r="K435" s="3"/>
     </row>
@@ -6959,7 +6966,6 @@
       <c r="F436" s="3"/>
       <c r="G436" s="3"/>
       <c r="H436" s="3"/>
-      <c r="I436" s="3"/>
       <c r="J436" s="3"/>
       <c r="K436" s="3"/>
     </row>
@@ -6984,6 +6990,7 @@
       <c r="F438" s="3"/>
       <c r="G438" s="3"/>
       <c r="H438" s="3"/>
+      <c r="I438" s="3"/>
       <c r="J438" s="3"/>
       <c r="K438" s="3"/>
     </row>
@@ -7035,7 +7042,6 @@
       <c r="F442" s="3"/>
       <c r="G442" s="3"/>
       <c r="H442" s="3"/>
-      <c r="I442" s="3"/>
       <c r="J442" s="3"/>
       <c r="K442" s="3"/>
     </row>
@@ -7048,6 +7054,7 @@
       <c r="F443" s="3"/>
       <c r="G443" s="3"/>
       <c r="H443" s="3"/>
+      <c r="I443" s="3"/>
       <c r="J443" s="3"/>
       <c r="K443" s="3"/>
     </row>
@@ -7099,7 +7106,6 @@
       <c r="F447" s="3"/>
       <c r="G447" s="3"/>
       <c r="H447" s="3"/>
-      <c r="I447" s="3"/>
       <c r="J447" s="3"/>
       <c r="K447" s="3"/>
     </row>
@@ -7112,6 +7118,7 @@
       <c r="F448" s="3"/>
       <c r="G448" s="3"/>
       <c r="H448" s="3"/>
+      <c r="I448" s="3"/>
       <c r="J448" s="3"/>
       <c r="K448" s="3"/>
     </row>
@@ -7228,7 +7235,6 @@
       <c r="F457" s="3"/>
       <c r="G457" s="3"/>
       <c r="H457" s="3"/>
-      <c r="I457" s="3"/>
       <c r="J457" s="3"/>
       <c r="K457" s="3"/>
     </row>
@@ -7241,6 +7247,7 @@
       <c r="F458" s="3"/>
       <c r="G458" s="3"/>
       <c r="H458" s="3"/>
+      <c r="I458" s="3"/>
       <c r="J458" s="3"/>
       <c r="K458" s="3"/>
     </row>
@@ -7253,7 +7260,6 @@
       <c r="F459" s="3"/>
       <c r="G459" s="3"/>
       <c r="H459" s="3"/>
-      <c r="I459" s="3"/>
       <c r="J459" s="3"/>
       <c r="K459" s="3"/>
     </row>
@@ -7266,6 +7272,7 @@
       <c r="F460" s="3"/>
       <c r="G460" s="3"/>
       <c r="H460" s="3"/>
+      <c r="I460" s="3"/>
       <c r="J460" s="3"/>
       <c r="K460" s="3"/>
     </row>
@@ -7343,7 +7350,6 @@
       <c r="F466" s="3"/>
       <c r="G466" s="3"/>
       <c r="H466" s="3"/>
-      <c r="I466" s="3"/>
       <c r="J466" s="3"/>
       <c r="K466" s="3"/>
     </row>
@@ -7356,6 +7362,7 @@
       <c r="F467" s="3"/>
       <c r="G467" s="3"/>
       <c r="H467" s="3"/>
+      <c r="I467" s="3"/>
       <c r="J467" s="3"/>
       <c r="K467" s="3"/>
     </row>
@@ -7394,7 +7401,6 @@
       <c r="F470" s="3"/>
       <c r="G470" s="3"/>
       <c r="H470" s="3"/>
-      <c r="I470" s="3"/>
       <c r="J470" s="3"/>
       <c r="K470" s="3"/>
     </row>
@@ -7407,6 +7413,7 @@
       <c r="F471" s="3"/>
       <c r="G471" s="3"/>
       <c r="H471" s="3"/>
+      <c r="I471" s="3"/>
       <c r="J471" s="3"/>
       <c r="K471" s="3"/>
     </row>
@@ -7483,7 +7490,6 @@
       <c r="E477" s="3"/>
       <c r="F477" s="3"/>
       <c r="G477" s="3"/>
-      <c r="H477" s="3"/>
       <c r="I477" s="3"/>
       <c r="J477" s="3"/>
       <c r="K477" s="3"/>
@@ -7496,7 +7502,7 @@
       <c r="E478" s="3"/>
       <c r="F478" s="3"/>
       <c r="G478" s="3"/>
-      <c r="I478" s="3"/>
+      <c r="H478" s="3"/>
       <c r="J478" s="3"/>
       <c r="K478" s="3"/>
     </row>
@@ -7509,6 +7515,7 @@
       <c r="F479" s="3"/>
       <c r="G479" s="3"/>
       <c r="H479" s="3"/>
+      <c r="I479" s="3"/>
       <c r="J479" s="3"/>
       <c r="K479" s="3"/>
     </row>
@@ -7547,7 +7554,6 @@
       <c r="F482" s="3"/>
       <c r="G482" s="3"/>
       <c r="H482" s="3"/>
-      <c r="I482" s="3"/>
       <c r="J482" s="3"/>
       <c r="K482" s="3"/>
     </row>
@@ -7560,6 +7566,7 @@
       <c r="F483" s="3"/>
       <c r="G483" s="3"/>
       <c r="H483" s="3"/>
+      <c r="I483" s="3"/>
       <c r="J483" s="3"/>
       <c r="K483" s="3"/>
     </row>
@@ -7611,7 +7618,6 @@
       <c r="F487" s="3"/>
       <c r="G487" s="3"/>
       <c r="H487" s="3"/>
-      <c r="I487" s="3"/>
       <c r="J487" s="3"/>
       <c r="K487" s="3"/>
     </row>
@@ -7648,6 +7654,7 @@
       <c r="F490" s="3"/>
       <c r="G490" s="3"/>
       <c r="H490" s="3"/>
+      <c r="I490" s="3"/>
       <c r="J490" s="3"/>
       <c r="K490" s="3"/>
     </row>
@@ -7725,7 +7732,6 @@
       <c r="F496" s="3"/>
       <c r="G496" s="3"/>
       <c r="H496" s="3"/>
-      <c r="I496" s="3"/>
       <c r="J496" s="3"/>
       <c r="K496" s="3"/>
     </row>
@@ -7750,6 +7756,7 @@
       <c r="F498" s="3"/>
       <c r="G498" s="3"/>
       <c r="H498" s="3"/>
+      <c r="I498" s="3"/>
       <c r="J498" s="3"/>
       <c r="K498" s="3"/>
     </row>
@@ -8008,7 +8015,6 @@
       <c r="E518" s="3"/>
       <c r="F518" s="3"/>
       <c r="G518" s="3"/>
-      <c r="H518" s="3"/>
       <c r="I518" s="3"/>
       <c r="J518" s="3"/>
       <c r="K518" s="3"/>
@@ -8021,6 +8027,7 @@
       <c r="E519" s="3"/>
       <c r="F519" s="3"/>
       <c r="G519" s="3"/>
+      <c r="H519" s="3"/>
       <c r="I519" s="3"/>
       <c r="J519" s="3"/>
       <c r="K519" s="3"/>
@@ -8033,7 +8040,6 @@
       <c r="E520" s="3"/>
       <c r="F520" s="3"/>
       <c r="G520" s="3"/>
-      <c r="H520" s="3"/>
       <c r="I520" s="3"/>
       <c r="J520" s="3"/>
       <c r="K520" s="3"/>
@@ -8046,6 +8052,7 @@
       <c r="E521" s="3"/>
       <c r="F521" s="3"/>
       <c r="G521" s="3"/>
+      <c r="H521" s="3"/>
       <c r="I521" s="3"/>
       <c r="J521" s="3"/>
       <c r="K521" s="3"/>
@@ -8461,7 +8468,6 @@
       <c r="E553" s="3"/>
       <c r="F553" s="3"/>
       <c r="G553" s="3"/>
-      <c r="H553" s="3"/>
       <c r="I553" s="3"/>
       <c r="J553" s="3"/>
       <c r="K553" s="3"/>
@@ -8474,6 +8480,7 @@
       <c r="E554" s="3"/>
       <c r="F554" s="3"/>
       <c r="G554" s="3"/>
+      <c r="H554" s="3"/>
       <c r="I554" s="3"/>
       <c r="J554" s="3"/>
       <c r="K554" s="3"/>
@@ -8603,7 +8610,6 @@
       <c r="E564" s="3"/>
       <c r="F564" s="3"/>
       <c r="G564" s="3"/>
-      <c r="H564" s="3"/>
       <c r="I564" s="3"/>
       <c r="J564" s="3"/>
       <c r="K564" s="3"/>
@@ -8616,6 +8622,7 @@
       <c r="E565" s="3"/>
       <c r="F565" s="3"/>
       <c r="G565" s="3"/>
+      <c r="H565" s="3"/>
       <c r="I565" s="3"/>
       <c r="J565" s="3"/>
       <c r="K565" s="3"/>
@@ -8758,7 +8765,6 @@
       <c r="E576" s="3"/>
       <c r="F576" s="3"/>
       <c r="G576" s="3"/>
-      <c r="H576" s="3"/>
       <c r="I576" s="3"/>
       <c r="J576" s="3"/>
       <c r="K576" s="3"/>
@@ -8771,6 +8777,7 @@
       <c r="E577" s="3"/>
       <c r="F577" s="3"/>
       <c r="G577" s="3"/>
+      <c r="H577" s="3"/>
       <c r="I577" s="3"/>
       <c r="J577" s="3"/>
       <c r="K577" s="3"/>
@@ -8861,7 +8868,6 @@
       <c r="E584" s="3"/>
       <c r="F584" s="3"/>
       <c r="G584" s="3"/>
-      <c r="H584" s="3"/>
       <c r="I584" s="3"/>
       <c r="J584" s="3"/>
       <c r="K584" s="3"/>
@@ -8874,6 +8880,7 @@
       <c r="E585" s="3"/>
       <c r="F585" s="3"/>
       <c r="G585" s="3"/>
+      <c r="H585" s="3"/>
       <c r="I585" s="3"/>
       <c r="J585" s="3"/>
       <c r="K585" s="3"/>
@@ -8912,7 +8919,6 @@
       <c r="E588" s="3"/>
       <c r="F588" s="3"/>
       <c r="G588" s="3"/>
-      <c r="H588" s="3"/>
       <c r="I588" s="3"/>
       <c r="J588" s="3"/>
       <c r="K588" s="3"/>
@@ -8925,6 +8931,7 @@
       <c r="E589" s="3"/>
       <c r="F589" s="3"/>
       <c r="G589" s="3"/>
+      <c r="H589" s="3"/>
       <c r="I589" s="3"/>
       <c r="J589" s="3"/>
       <c r="K589" s="3"/>
@@ -8937,7 +8944,6 @@
       <c r="E590" s="3"/>
       <c r="F590" s="3"/>
       <c r="G590" s="3"/>
-      <c r="H590" s="3"/>
       <c r="I590" s="3"/>
       <c r="J590" s="3"/>
       <c r="K590" s="3"/>
@@ -8950,6 +8956,7 @@
       <c r="E591" s="3"/>
       <c r="F591" s="3"/>
       <c r="G591" s="3"/>
+      <c r="H591" s="3"/>
       <c r="I591" s="3"/>
       <c r="J591" s="3"/>
       <c r="K591" s="3"/>
@@ -9001,7 +9008,6 @@
       <c r="E595" s="3"/>
       <c r="F595" s="3"/>
       <c r="G595" s="3"/>
-      <c r="H595" s="3"/>
       <c r="I595" s="3"/>
       <c r="J595" s="3"/>
       <c r="K595" s="3"/>
@@ -9014,6 +9020,7 @@
       <c r="E596" s="3"/>
       <c r="F596" s="3"/>
       <c r="G596" s="3"/>
+      <c r="H596" s="3"/>
       <c r="I596" s="3"/>
       <c r="J596" s="3"/>
       <c r="K596" s="3"/>
@@ -9052,7 +9059,6 @@
       <c r="E599" s="3"/>
       <c r="F599" s="3"/>
       <c r="G599" s="3"/>
-      <c r="H599" s="3"/>
       <c r="I599" s="3"/>
       <c r="J599" s="3"/>
       <c r="K599" s="3"/>
@@ -9078,7 +9084,6 @@
       <c r="F601" s="3"/>
       <c r="G601" s="3"/>
       <c r="I601" s="3"/>
-      <c r="J601" s="3"/>
       <c r="K601" s="3"/>
     </row>
     <row r="602" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9100,6 +9105,7 @@
       <c r="E603" s="3"/>
       <c r="F603" s="3"/>
       <c r="G603" s="3"/>
+      <c r="H603" s="3"/>
       <c r="I603" s="3"/>
       <c r="K603" s="3"/>
     </row>
@@ -9137,6 +9143,7 @@
       <c r="G606" s="3"/>
       <c r="H606" s="3"/>
       <c r="I606" s="3"/>
+      <c r="J606" s="3"/>
       <c r="K606" s="3"/>
     </row>
     <row r="607" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9161,7 +9168,6 @@
       <c r="F608" s="3"/>
       <c r="G608" s="3"/>
       <c r="H608" s="3"/>
-      <c r="I608" s="3"/>
       <c r="J608" s="3"/>
       <c r="K608" s="3"/>
     </row>
@@ -9222,6 +9228,7 @@
       <c r="F613" s="3"/>
       <c r="G613" s="3"/>
       <c r="H613" s="3"/>
+      <c r="I613" s="3"/>
       <c r="J613" s="3"/>
       <c r="K613" s="3"/>
     </row>
@@ -9234,7 +9241,6 @@
       <c r="F614" s="3"/>
       <c r="G614" s="3"/>
       <c r="H614" s="3"/>
-      <c r="I614" s="3"/>
       <c r="J614" s="3"/>
       <c r="K614" s="3"/>
     </row>
@@ -9247,6 +9253,7 @@
       <c r="F615" s="3"/>
       <c r="G615" s="3"/>
       <c r="H615" s="3"/>
+      <c r="I615" s="3"/>
       <c r="J615" s="3"/>
       <c r="K615" s="3"/>
     </row>
@@ -9298,7 +9305,6 @@
       <c r="F619" s="3"/>
       <c r="G619" s="3"/>
       <c r="H619" s="3"/>
-      <c r="I619" s="3"/>
       <c r="J619" s="3"/>
       <c r="K619" s="3"/>
     </row>
@@ -9311,6 +9317,7 @@
       <c r="F620" s="3"/>
       <c r="G620" s="3"/>
       <c r="H620" s="3"/>
+      <c r="I620" s="3"/>
       <c r="J620" s="3"/>
       <c r="K620" s="3"/>
     </row>
@@ -9362,7 +9369,6 @@
       <c r="F624" s="3"/>
       <c r="G624" s="3"/>
       <c r="H624" s="3"/>
-      <c r="I624" s="3"/>
       <c r="J624" s="3"/>
       <c r="K624" s="3"/>
     </row>
@@ -9375,6 +9381,7 @@
       <c r="F625" s="3"/>
       <c r="G625" s="3"/>
       <c r="H625" s="3"/>
+      <c r="I625" s="3"/>
       <c r="J625" s="3"/>
       <c r="K625" s="3"/>
     </row>
@@ -9400,7 +9407,6 @@
       <c r="F627" s="3"/>
       <c r="G627" s="3"/>
       <c r="H627" s="3"/>
-      <c r="I627" s="3"/>
       <c r="J627" s="3"/>
       <c r="K627" s="3"/>
     </row>
@@ -9413,6 +9419,7 @@
       <c r="F628" s="3"/>
       <c r="G628" s="3"/>
       <c r="H628" s="3"/>
+      <c r="I628" s="3"/>
       <c r="J628" s="3"/>
       <c r="K628" s="3"/>
     </row>
@@ -9425,7 +9432,6 @@
       <c r="F629" s="3"/>
       <c r="G629" s="3"/>
       <c r="H629" s="3"/>
-      <c r="I629" s="3"/>
       <c r="J629" s="3"/>
       <c r="K629" s="3"/>
     </row>
@@ -9450,6 +9456,7 @@
       <c r="F631" s="3"/>
       <c r="G631" s="3"/>
       <c r="H631" s="3"/>
+      <c r="I631" s="3"/>
       <c r="J631" s="3"/>
       <c r="K631" s="3"/>
     </row>
@@ -9488,7 +9495,6 @@
       <c r="F634" s="3"/>
       <c r="G634" s="3"/>
       <c r="H634" s="3"/>
-      <c r="I634" s="3"/>
       <c r="J634" s="3"/>
       <c r="K634" s="3"/>
     </row>
@@ -9501,6 +9507,7 @@
       <c r="F635" s="3"/>
       <c r="G635" s="3"/>
       <c r="H635" s="3"/>
+      <c r="I635" s="3"/>
       <c r="J635" s="3"/>
       <c r="K635" s="3"/>
     </row>
@@ -9539,7 +9546,6 @@
       <c r="F638" s="3"/>
       <c r="G638" s="3"/>
       <c r="H638" s="3"/>
-      <c r="I638" s="3"/>
       <c r="J638" s="3"/>
       <c r="K638" s="3"/>
     </row>
@@ -9564,6 +9570,7 @@
       <c r="F640" s="3"/>
       <c r="G640" s="3"/>
       <c r="H640" s="3"/>
+      <c r="I640" s="3"/>
       <c r="J640" s="3"/>
       <c r="K640" s="3"/>
     </row>
@@ -9615,7 +9622,6 @@
       <c r="F644" s="3"/>
       <c r="G644" s="3"/>
       <c r="H644" s="3"/>
-      <c r="I644" s="3"/>
       <c r="J644" s="3"/>
       <c r="K644" s="3"/>
     </row>
@@ -9628,6 +9634,7 @@
       <c r="F645" s="3"/>
       <c r="G645" s="3"/>
       <c r="H645" s="3"/>
+      <c r="I645" s="3"/>
       <c r="J645" s="3"/>
       <c r="K645" s="3"/>
     </row>
@@ -9705,7 +9712,6 @@
       <c r="F651" s="3"/>
       <c r="G651" s="3"/>
       <c r="H651" s="3"/>
-      <c r="I651" s="3"/>
       <c r="J651" s="3"/>
       <c r="K651" s="3"/>
     </row>
@@ -9730,6 +9736,7 @@
       <c r="F653" s="3"/>
       <c r="G653" s="3"/>
       <c r="H653" s="3"/>
+      <c r="I653" s="3"/>
       <c r="J653" s="3"/>
       <c r="K653" s="3"/>
     </row>
@@ -9742,7 +9749,6 @@
       <c r="F654" s="3"/>
       <c r="G654" s="3"/>
       <c r="H654" s="3"/>
-      <c r="I654" s="3"/>
       <c r="J654" s="3"/>
       <c r="K654" s="3"/>
     </row>
@@ -9755,6 +9761,7 @@
       <c r="F655" s="3"/>
       <c r="G655" s="3"/>
       <c r="H655" s="3"/>
+      <c r="I655" s="3"/>
       <c r="J655" s="3"/>
       <c r="K655" s="3"/>
     </row>
@@ -9780,7 +9787,6 @@
       <c r="F657" s="3"/>
       <c r="G657" s="3"/>
       <c r="H657" s="3"/>
-      <c r="I657" s="3"/>
       <c r="J657" s="3"/>
       <c r="K657" s="3"/>
     </row>
@@ -9793,6 +9799,7 @@
       <c r="F658" s="3"/>
       <c r="G658" s="3"/>
       <c r="H658" s="3"/>
+      <c r="I658" s="3"/>
       <c r="J658" s="3"/>
       <c r="K658" s="3"/>
     </row>
@@ -9818,7 +9825,6 @@
       <c r="F660" s="3"/>
       <c r="G660" s="3"/>
       <c r="H660" s="3"/>
-      <c r="I660" s="3"/>
       <c r="J660" s="3"/>
       <c r="K660" s="3"/>
     </row>
@@ -9855,6 +9861,7 @@
       <c r="F663" s="3"/>
       <c r="G663" s="3"/>
       <c r="H663" s="3"/>
+      <c r="I663" s="3"/>
       <c r="J663" s="3"/>
       <c r="K663" s="3"/>
     </row>
@@ -9984,7 +9991,6 @@
       <c r="F673" s="3"/>
       <c r="G673" s="3"/>
       <c r="H673" s="3"/>
-      <c r="I673" s="3"/>
       <c r="J673" s="3"/>
       <c r="K673" s="3"/>
     </row>
@@ -9997,6 +10003,7 @@
       <c r="F674" s="3"/>
       <c r="G674" s="3"/>
       <c r="H674" s="3"/>
+      <c r="I674" s="3"/>
       <c r="J674" s="3"/>
       <c r="K674" s="3"/>
     </row>
@@ -10009,7 +10016,6 @@
       <c r="F675" s="3"/>
       <c r="G675" s="3"/>
       <c r="H675" s="3"/>
-      <c r="I675" s="3"/>
       <c r="J675" s="3"/>
       <c r="K675" s="3"/>
     </row>
@@ -10022,6 +10028,7 @@
       <c r="F676" s="3"/>
       <c r="G676" s="3"/>
       <c r="H676" s="3"/>
+      <c r="I676" s="3"/>
       <c r="J676" s="3"/>
       <c r="K676" s="3"/>
     </row>
@@ -10073,7 +10080,6 @@
       <c r="F680" s="3"/>
       <c r="G680" s="3"/>
       <c r="H680" s="3"/>
-      <c r="I680" s="3"/>
       <c r="J680" s="3"/>
       <c r="K680" s="3"/>
     </row>
@@ -10086,6 +10092,7 @@
       <c r="F681" s="3"/>
       <c r="G681" s="3"/>
       <c r="H681" s="3"/>
+      <c r="I681" s="3"/>
       <c r="J681" s="3"/>
       <c r="K681" s="3"/>
     </row>
@@ -10137,7 +10144,6 @@
       <c r="F685" s="3"/>
       <c r="G685" s="3"/>
       <c r="H685" s="3"/>
-      <c r="I685" s="3"/>
       <c r="J685" s="3"/>
       <c r="K685" s="3"/>
     </row>
@@ -10150,6 +10156,7 @@
       <c r="F686" s="3"/>
       <c r="G686" s="3"/>
       <c r="H686" s="3"/>
+      <c r="I686" s="3"/>
       <c r="J686" s="3"/>
       <c r="K686" s="3"/>
     </row>
@@ -10214,7 +10221,6 @@
       <c r="F691" s="3"/>
       <c r="G691" s="3"/>
       <c r="H691" s="3"/>
-      <c r="I691" s="3"/>
       <c r="J691" s="3"/>
       <c r="K691" s="3"/>
     </row>
@@ -10239,6 +10245,7 @@
       <c r="F693" s="3"/>
       <c r="G693" s="3"/>
       <c r="H693" s="3"/>
+      <c r="I693" s="3"/>
       <c r="J693" s="3"/>
       <c r="K693" s="3"/>
     </row>
@@ -10277,7 +10284,6 @@
       <c r="F696" s="3"/>
       <c r="G696" s="3"/>
       <c r="H696" s="3"/>
-      <c r="I696" s="3"/>
       <c r="J696" s="3"/>
       <c r="K696" s="3"/>
     </row>
@@ -10290,6 +10296,7 @@
       <c r="F697" s="3"/>
       <c r="G697" s="3"/>
       <c r="H697" s="3"/>
+      <c r="I697" s="3"/>
       <c r="J697" s="3"/>
       <c r="K697" s="3"/>
     </row>
@@ -10315,7 +10322,6 @@
       <c r="F699" s="3"/>
       <c r="G699" s="3"/>
       <c r="H699" s="3"/>
-      <c r="I699" s="3"/>
       <c r="J699" s="3"/>
       <c r="K699" s="3"/>
     </row>
@@ -10328,6 +10334,7 @@
       <c r="F700" s="3"/>
       <c r="G700" s="3"/>
       <c r="H700" s="3"/>
+      <c r="I700" s="3"/>
       <c r="J700" s="3"/>
       <c r="K700" s="3"/>
     </row>
@@ -10353,7 +10360,6 @@
       <c r="F702" s="3"/>
       <c r="G702" s="3"/>
       <c r="H702" s="3"/>
-      <c r="I702" s="3"/>
       <c r="J702" s="3"/>
       <c r="K702" s="3"/>
     </row>
@@ -10366,6 +10372,7 @@
       <c r="F703" s="3"/>
       <c r="G703" s="3"/>
       <c r="H703" s="3"/>
+      <c r="I703" s="3"/>
       <c r="J703" s="3"/>
       <c r="K703" s="3"/>
     </row>
@@ -10430,7 +10437,6 @@
       <c r="F708" s="3"/>
       <c r="G708" s="3"/>
       <c r="H708" s="3"/>
-      <c r="I708" s="3"/>
       <c r="J708" s="3"/>
       <c r="K708" s="3"/>
     </row>
@@ -10443,6 +10449,7 @@
       <c r="F709" s="3"/>
       <c r="G709" s="3"/>
       <c r="H709" s="3"/>
+      <c r="I709" s="3"/>
       <c r="J709" s="3"/>
       <c r="K709" s="3"/>
     </row>
@@ -10455,7 +10462,6 @@
       <c r="F710" s="3"/>
       <c r="G710" s="3"/>
       <c r="H710" s="3"/>
-      <c r="I710" s="3"/>
       <c r="J710" s="3"/>
       <c r="K710" s="3"/>
     </row>
@@ -10468,6 +10474,7 @@
       <c r="F711" s="3"/>
       <c r="G711" s="3"/>
       <c r="H711" s="3"/>
+      <c r="I711" s="3"/>
       <c r="J711" s="3"/>
       <c r="K711" s="3"/>
     </row>
@@ -10493,7 +10500,6 @@
       <c r="F713" s="3"/>
       <c r="G713" s="3"/>
       <c r="H713" s="3"/>
-      <c r="I713" s="3"/>
       <c r="J713" s="3"/>
       <c r="K713" s="3"/>
     </row>
@@ -10530,6 +10536,7 @@
       <c r="F716" s="3"/>
       <c r="G716" s="3"/>
       <c r="H716" s="3"/>
+      <c r="I716" s="3"/>
       <c r="J716" s="3"/>
       <c r="K716" s="3"/>
     </row>
@@ -10542,7 +10549,6 @@
       <c r="F717" s="3"/>
       <c r="G717" s="3"/>
       <c r="H717" s="3"/>
-      <c r="I717" s="3"/>
       <c r="J717" s="3"/>
       <c r="K717" s="3"/>
     </row>
@@ -10567,6 +10573,7 @@
       <c r="F719" s="3"/>
       <c r="G719" s="3"/>
       <c r="H719" s="3"/>
+      <c r="I719" s="3"/>
       <c r="J719" s="3"/>
       <c r="K719" s="3"/>
     </row>
@@ -10605,7 +10612,6 @@
       <c r="F722" s="3"/>
       <c r="G722" s="3"/>
       <c r="H722" s="3"/>
-      <c r="I722" s="3"/>
       <c r="J722" s="3"/>
       <c r="K722" s="3"/>
     </row>
@@ -10618,6 +10624,7 @@
       <c r="F723" s="3"/>
       <c r="G723" s="3"/>
       <c r="H723" s="3"/>
+      <c r="I723" s="3"/>
       <c r="J723" s="3"/>
       <c r="K723" s="3"/>
     </row>
@@ -10643,7 +10650,6 @@
       <c r="F725" s="3"/>
       <c r="G725" s="3"/>
       <c r="H725" s="3"/>
-      <c r="I725" s="3"/>
       <c r="J725" s="3"/>
       <c r="K725" s="3"/>
     </row>
@@ -10656,6 +10662,7 @@
       <c r="F726" s="3"/>
       <c r="G726" s="3"/>
       <c r="H726" s="3"/>
+      <c r="I726" s="3"/>
       <c r="J726" s="3"/>
       <c r="K726" s="3"/>
     </row>
@@ -10733,7 +10740,6 @@
       <c r="F732" s="3"/>
       <c r="G732" s="3"/>
       <c r="H732" s="3"/>
-      <c r="I732" s="3"/>
       <c r="J732" s="3"/>
       <c r="K732" s="3"/>
     </row>
@@ -10758,6 +10764,7 @@
       <c r="F734" s="3"/>
       <c r="G734" s="3"/>
       <c r="H734" s="3"/>
+      <c r="I734" s="3"/>
       <c r="J734" s="3"/>
       <c r="K734" s="3"/>
     </row>
@@ -10770,7 +10777,6 @@
       <c r="F735" s="3"/>
       <c r="G735" s="3"/>
       <c r="H735" s="3"/>
-      <c r="I735" s="3"/>
       <c r="J735" s="3"/>
       <c r="K735" s="3"/>
     </row>
@@ -10783,6 +10789,7 @@
       <c r="F736" s="3"/>
       <c r="G736" s="3"/>
       <c r="H736" s="3"/>
+      <c r="I736" s="3"/>
       <c r="J736" s="3"/>
       <c r="K736" s="3"/>
     </row>
@@ -10821,7 +10828,6 @@
       <c r="F739" s="3"/>
       <c r="G739" s="3"/>
       <c r="H739" s="3"/>
-      <c r="I739" s="3"/>
       <c r="J739" s="3"/>
       <c r="K739" s="3"/>
     </row>
@@ -10846,6 +10852,7 @@
       <c r="F741" s="3"/>
       <c r="G741" s="3"/>
       <c r="H741" s="3"/>
+      <c r="I741" s="3"/>
       <c r="J741" s="3"/>
       <c r="K741" s="3"/>
     </row>
@@ -10858,7 +10865,6 @@
       <c r="F742" s="3"/>
       <c r="G742" s="3"/>
       <c r="H742" s="3"/>
-      <c r="I742" s="3"/>
       <c r="J742" s="3"/>
       <c r="K742" s="3"/>
     </row>
@@ -10871,6 +10877,7 @@
       <c r="F743" s="3"/>
       <c r="G743" s="3"/>
       <c r="H743" s="3"/>
+      <c r="I743" s="3"/>
       <c r="J743" s="3"/>
       <c r="K743" s="3"/>
     </row>
@@ -10922,7 +10929,6 @@
       <c r="F747" s="3"/>
       <c r="G747" s="3"/>
       <c r="H747" s="3"/>
-      <c r="I747" s="3"/>
       <c r="J747" s="3"/>
       <c r="K747" s="3"/>
     </row>
@@ -10935,6 +10941,7 @@
       <c r="F748" s="3"/>
       <c r="G748" s="3"/>
       <c r="H748" s="3"/>
+      <c r="I748" s="3"/>
       <c r="J748" s="3"/>
       <c r="K748" s="3"/>
     </row>
@@ -10947,7 +10954,6 @@
       <c r="F749" s="3"/>
       <c r="G749" s="3"/>
       <c r="H749" s="3"/>
-      <c r="I749" s="3"/>
       <c r="J749" s="3"/>
       <c r="K749" s="3"/>
     </row>
@@ -10960,6 +10966,7 @@
       <c r="F750" s="3"/>
       <c r="G750" s="3"/>
       <c r="H750" s="3"/>
+      <c r="I750" s="3"/>
       <c r="J750" s="3"/>
       <c r="K750" s="3"/>
     </row>
@@ -10985,7 +10992,6 @@
       <c r="F752" s="3"/>
       <c r="G752" s="3"/>
       <c r="H752" s="3"/>
-      <c r="I752" s="3"/>
       <c r="J752" s="3"/>
       <c r="K752" s="3"/>
     </row>
@@ -10998,6 +11004,7 @@
       <c r="F753" s="3"/>
       <c r="G753" s="3"/>
       <c r="H753" s="3"/>
+      <c r="I753" s="3"/>
       <c r="J753" s="3"/>
       <c r="K753" s="3"/>
     </row>
@@ -11023,7 +11030,6 @@
       <c r="F755" s="3"/>
       <c r="G755" s="3"/>
       <c r="H755" s="3"/>
-      <c r="I755" s="3"/>
       <c r="J755" s="3"/>
       <c r="K755" s="3"/>
     </row>
@@ -11048,6 +11054,7 @@
       <c r="F757" s="3"/>
       <c r="G757" s="3"/>
       <c r="H757" s="3"/>
+      <c r="I757" s="3"/>
       <c r="J757" s="3"/>
       <c r="K757" s="3"/>
     </row>
@@ -11073,7 +11080,6 @@
       <c r="F759" s="3"/>
       <c r="G759" s="3"/>
       <c r="H759" s="3"/>
-      <c r="I759" s="3"/>
       <c r="J759" s="3"/>
       <c r="K759" s="3"/>
     </row>
@@ -11098,6 +11104,7 @@
       <c r="F761" s="3"/>
       <c r="G761" s="3"/>
       <c r="H761" s="3"/>
+      <c r="I761" s="3"/>
       <c r="J761" s="3"/>
       <c r="K761" s="3"/>
     </row>
@@ -11136,7 +11143,6 @@
       <c r="F764" s="3"/>
       <c r="G764" s="3"/>
       <c r="H764" s="3"/>
-      <c r="I764" s="3"/>
       <c r="J764" s="3"/>
       <c r="K764" s="3"/>
     </row>
@@ -11161,6 +11167,7 @@
       <c r="F766" s="3"/>
       <c r="G766" s="3"/>
       <c r="H766" s="3"/>
+      <c r="I766" s="3"/>
       <c r="J766" s="3"/>
       <c r="K766" s="3"/>
     </row>
@@ -11173,7 +11180,6 @@
       <c r="F767" s="3"/>
       <c r="G767" s="3"/>
       <c r="H767" s="3"/>
-      <c r="I767" s="3"/>
       <c r="J767" s="3"/>
       <c r="K767" s="3"/>
     </row>
@@ -11186,6 +11192,7 @@
       <c r="F768" s="3"/>
       <c r="G768" s="3"/>
       <c r="H768" s="3"/>
+      <c r="I768" s="3"/>
       <c r="J768" s="3"/>
       <c r="K768" s="3"/>
     </row>
@@ -11211,7 +11218,6 @@
       <c r="F770" s="3"/>
       <c r="G770" s="3"/>
       <c r="H770" s="3"/>
-      <c r="I770" s="3"/>
       <c r="J770" s="3"/>
       <c r="K770" s="3"/>
     </row>
@@ -11224,6 +11230,7 @@
       <c r="F771" s="3"/>
       <c r="G771" s="3"/>
       <c r="H771" s="3"/>
+      <c r="I771" s="3"/>
       <c r="J771" s="3"/>
       <c r="K771" s="3"/>
     </row>
@@ -11288,7 +11295,6 @@
       <c r="F776" s="3"/>
       <c r="G776" s="3"/>
       <c r="H776" s="3"/>
-      <c r="I776" s="3"/>
       <c r="J776" s="3"/>
       <c r="K776" s="3"/>
     </row>
@@ -11301,6 +11307,7 @@
       <c r="F777" s="3"/>
       <c r="G777" s="3"/>
       <c r="H777" s="3"/>
+      <c r="I777" s="3"/>
       <c r="J777" s="3"/>
       <c r="K777" s="3"/>
     </row>
@@ -11391,7 +11398,6 @@
       <c r="F784" s="3"/>
       <c r="G784" s="3"/>
       <c r="H784" s="3"/>
-      <c r="I784" s="3"/>
       <c r="J784" s="3"/>
       <c r="K784" s="3"/>
     </row>
@@ -11404,6 +11410,7 @@
       <c r="F785" s="3"/>
       <c r="G785" s="3"/>
       <c r="H785" s="3"/>
+      <c r="I785" s="3"/>
       <c r="J785" s="3"/>
       <c r="K785" s="3"/>
     </row>
@@ -11481,7 +11488,6 @@
       <c r="F791" s="3"/>
       <c r="G791" s="3"/>
       <c r="H791" s="3"/>
-      <c r="I791" s="3"/>
       <c r="J791" s="3"/>
       <c r="K791" s="3"/>
     </row>
@@ -11494,6 +11500,7 @@
       <c r="F792" s="3"/>
       <c r="G792" s="3"/>
       <c r="H792" s="3"/>
+      <c r="I792" s="3"/>
       <c r="J792" s="3"/>
       <c r="K792" s="3"/>
     </row>
@@ -11532,7 +11539,6 @@
       <c r="F795" s="3"/>
       <c r="G795" s="3"/>
       <c r="H795" s="3"/>
-      <c r="I795" s="3"/>
       <c r="J795" s="3"/>
       <c r="K795" s="3"/>
     </row>
@@ -11557,6 +11563,7 @@
       <c r="F797" s="3"/>
       <c r="G797" s="3"/>
       <c r="H797" s="3"/>
+      <c r="I797" s="3"/>
       <c r="J797" s="3"/>
       <c r="K797" s="3"/>
     </row>
@@ -11621,7 +11628,6 @@
       <c r="F802" s="3"/>
       <c r="G802" s="3"/>
       <c r="H802" s="3"/>
-      <c r="I802" s="3"/>
       <c r="J802" s="3"/>
       <c r="K802" s="3"/>
     </row>
@@ -11634,6 +11640,7 @@
       <c r="F803" s="3"/>
       <c r="G803" s="3"/>
       <c r="H803" s="3"/>
+      <c r="I803" s="3"/>
       <c r="J803" s="3"/>
       <c r="K803" s="3"/>
     </row>
@@ -11685,7 +11692,6 @@
       <c r="F807" s="3"/>
       <c r="G807" s="3"/>
       <c r="H807" s="3"/>
-      <c r="I807" s="3"/>
       <c r="J807" s="3"/>
       <c r="K807" s="3"/>
     </row>
@@ -11698,6 +11704,7 @@
       <c r="F808" s="3"/>
       <c r="G808" s="3"/>
       <c r="H808" s="3"/>
+      <c r="I808" s="3"/>
       <c r="J808" s="3"/>
       <c r="K808" s="3"/>
     </row>
@@ -11736,7 +11743,6 @@
       <c r="F811" s="3"/>
       <c r="G811" s="3"/>
       <c r="H811" s="3"/>
-      <c r="I811" s="3"/>
       <c r="J811" s="3"/>
       <c r="K811" s="3"/>
     </row>
@@ -11749,6 +11755,7 @@
       <c r="F812" s="3"/>
       <c r="G812" s="3"/>
       <c r="H812" s="3"/>
+      <c r="I812" s="3"/>
       <c r="J812" s="3"/>
       <c r="K812" s="3"/>
     </row>
@@ -11774,7 +11781,6 @@
       <c r="F814" s="3"/>
       <c r="G814" s="3"/>
       <c r="H814" s="3"/>
-      <c r="I814" s="3"/>
       <c r="J814" s="3"/>
       <c r="K814" s="3"/>
     </row>
@@ -11787,6 +11793,7 @@
       <c r="F815" s="3"/>
       <c r="G815" s="3"/>
       <c r="H815" s="3"/>
+      <c r="I815" s="3"/>
       <c r="J815" s="3"/>
       <c r="K815" s="3"/>
     </row>
@@ -11812,7 +11819,6 @@
       <c r="F817" s="3"/>
       <c r="G817" s="3"/>
       <c r="H817" s="3"/>
-      <c r="I817" s="3"/>
       <c r="J817" s="3"/>
       <c r="K817" s="3"/>
     </row>
@@ -11825,6 +11831,7 @@
       <c r="F818" s="3"/>
       <c r="G818" s="3"/>
       <c r="H818" s="3"/>
+      <c r="I818" s="3"/>
       <c r="J818" s="3"/>
       <c r="K818" s="3"/>
     </row>
@@ -11876,7 +11883,6 @@
       <c r="F822" s="3"/>
       <c r="G822" s="3"/>
       <c r="H822" s="3"/>
-      <c r="I822" s="3"/>
       <c r="J822" s="3"/>
       <c r="K822" s="3"/>
     </row>
@@ -11889,6 +11895,7 @@
       <c r="F823" s="3"/>
       <c r="G823" s="3"/>
       <c r="H823" s="3"/>
+      <c r="I823" s="3"/>
       <c r="J823" s="3"/>
       <c r="K823" s="3"/>
     </row>
@@ -11927,7 +11934,6 @@
       <c r="F826" s="3"/>
       <c r="G826" s="3"/>
       <c r="H826" s="3"/>
-      <c r="I826" s="3"/>
       <c r="J826" s="3"/>
       <c r="K826" s="3"/>
     </row>
@@ -11940,6 +11946,7 @@
       <c r="F827" s="3"/>
       <c r="G827" s="3"/>
       <c r="H827" s="3"/>
+      <c r="I827" s="3"/>
       <c r="J827" s="3"/>
       <c r="K827" s="3"/>
     </row>
@@ -11991,7 +11998,6 @@
       <c r="F831" s="3"/>
       <c r="G831" s="3"/>
       <c r="H831" s="3"/>
-      <c r="I831" s="3"/>
       <c r="J831" s="3"/>
       <c r="K831" s="3"/>
     </row>
@@ -12004,6 +12010,7 @@
       <c r="F832" s="3"/>
       <c r="G832" s="3"/>
       <c r="H832" s="3"/>
+      <c r="I832" s="3"/>
       <c r="J832" s="3"/>
       <c r="K832" s="3"/>
     </row>
@@ -12042,7 +12049,6 @@
       <c r="F835" s="3"/>
       <c r="G835" s="3"/>
       <c r="H835" s="3"/>
-      <c r="I835" s="3"/>
       <c r="J835" s="3"/>
       <c r="K835" s="3"/>
     </row>
@@ -12055,6 +12061,7 @@
       <c r="F836" s="3"/>
       <c r="G836" s="3"/>
       <c r="H836" s="3"/>
+      <c r="I836" s="3"/>
       <c r="J836" s="3"/>
       <c r="K836" s="3"/>
     </row>
@@ -12067,7 +12074,6 @@
       <c r="F837" s="3"/>
       <c r="G837" s="3"/>
       <c r="H837" s="3"/>
-      <c r="I837" s="3"/>
       <c r="J837" s="3"/>
       <c r="K837" s="3"/>
     </row>
@@ -12092,6 +12098,7 @@
       <c r="F839" s="3"/>
       <c r="G839" s="3"/>
       <c r="H839" s="3"/>
+      <c r="I839" s="3"/>
       <c r="J839" s="3"/>
       <c r="K839" s="3"/>
     </row>
@@ -12130,7 +12137,6 @@
       <c r="F842" s="3"/>
       <c r="G842" s="3"/>
       <c r="H842" s="3"/>
-      <c r="I842" s="3"/>
       <c r="J842" s="3"/>
       <c r="K842" s="3"/>
     </row>
@@ -12155,6 +12161,7 @@
       <c r="F844" s="3"/>
       <c r="G844" s="3"/>
       <c r="H844" s="3"/>
+      <c r="I844" s="3"/>
       <c r="J844" s="3"/>
       <c r="K844" s="3"/>
     </row>
@@ -12167,7 +12174,6 @@
       <c r="F845" s="3"/>
       <c r="G845" s="3"/>
       <c r="H845" s="3"/>
-      <c r="I845" s="3"/>
       <c r="J845" s="3"/>
       <c r="K845" s="3"/>
     </row>
@@ -12180,6 +12186,7 @@
       <c r="F846" s="3"/>
       <c r="G846" s="3"/>
       <c r="H846" s="3"/>
+      <c r="I846" s="3"/>
       <c r="J846" s="3"/>
       <c r="K846" s="3"/>
     </row>
@@ -12218,7 +12225,6 @@
       <c r="F849" s="3"/>
       <c r="G849" s="3"/>
       <c r="H849" s="3"/>
-      <c r="I849" s="3"/>
       <c r="J849" s="3"/>
       <c r="K849" s="3"/>
     </row>
@@ -12231,6 +12237,7 @@
       <c r="F850" s="3"/>
       <c r="G850" s="3"/>
       <c r="H850" s="3"/>
+      <c r="I850" s="3"/>
       <c r="J850" s="3"/>
       <c r="K850" s="3"/>
     </row>
@@ -12256,7 +12263,6 @@
       <c r="F852" s="3"/>
       <c r="G852" s="3"/>
       <c r="H852" s="3"/>
-      <c r="I852" s="3"/>
       <c r="J852" s="3"/>
       <c r="K852" s="3"/>
     </row>
@@ -12269,6 +12275,7 @@
       <c r="F853" s="3"/>
       <c r="G853" s="3"/>
       <c r="H853" s="3"/>
+      <c r="I853" s="3"/>
       <c r="J853" s="3"/>
       <c r="K853" s="3"/>
     </row>
@@ -12281,7 +12288,6 @@
       <c r="F854" s="3"/>
       <c r="G854" s="3"/>
       <c r="H854" s="3"/>
-      <c r="I854" s="3"/>
       <c r="J854" s="3"/>
       <c r="K854" s="3"/>
     </row>
@@ -12294,6 +12300,7 @@
       <c r="F855" s="3"/>
       <c r="G855" s="3"/>
       <c r="H855" s="3"/>
+      <c r="I855" s="3"/>
       <c r="J855" s="3"/>
       <c r="K855" s="3"/>
     </row>
@@ -12319,7 +12326,6 @@
       <c r="F857" s="3"/>
       <c r="G857" s="3"/>
       <c r="H857" s="3"/>
-      <c r="I857" s="3"/>
       <c r="J857" s="3"/>
       <c r="K857" s="3"/>
     </row>
@@ -12332,6 +12338,7 @@
       <c r="F858" s="3"/>
       <c r="G858" s="3"/>
       <c r="H858" s="3"/>
+      <c r="I858" s="3"/>
       <c r="J858" s="3"/>
       <c r="K858" s="3"/>
     </row>
@@ -12370,7 +12377,6 @@
       <c r="F861" s="3"/>
       <c r="G861" s="3"/>
       <c r="H861" s="3"/>
-      <c r="I861" s="3"/>
       <c r="J861" s="3"/>
       <c r="K861" s="3"/>
     </row>
@@ -12395,6 +12401,7 @@
       <c r="F863" s="3"/>
       <c r="G863" s="3"/>
       <c r="H863" s="3"/>
+      <c r="I863" s="3"/>
       <c r="J863" s="3"/>
       <c r="K863" s="3"/>
     </row>
@@ -12420,7 +12427,6 @@
       <c r="F865" s="3"/>
       <c r="G865" s="3"/>
       <c r="H865" s="3"/>
-      <c r="I865" s="3"/>
       <c r="J865" s="3"/>
       <c r="K865" s="3"/>
     </row>
@@ -12433,6 +12439,7 @@
       <c r="F866" s="3"/>
       <c r="G866" s="3"/>
       <c r="H866" s="3"/>
+      <c r="I866" s="3"/>
       <c r="J866" s="3"/>
       <c r="K866" s="3"/>
     </row>
@@ -12445,7 +12452,6 @@
       <c r="F867" s="3"/>
       <c r="G867" s="3"/>
       <c r="H867" s="3"/>
-      <c r="I867" s="3"/>
       <c r="J867" s="3"/>
       <c r="K867" s="3"/>
     </row>
@@ -12470,6 +12476,7 @@
       <c r="F869" s="3"/>
       <c r="G869" s="3"/>
       <c r="H869" s="3"/>
+      <c r="I869" s="3"/>
       <c r="J869" s="3"/>
       <c r="K869" s="3"/>
     </row>
@@ -12521,7 +12528,6 @@
       <c r="F873" s="3"/>
       <c r="G873" s="3"/>
       <c r="H873" s="3"/>
-      <c r="I873" s="3"/>
       <c r="J873" s="3"/>
       <c r="K873" s="3"/>
     </row>
@@ -12534,6 +12540,7 @@
       <c r="F874" s="3"/>
       <c r="G874" s="3"/>
       <c r="H874" s="3"/>
+      <c r="I874" s="3"/>
       <c r="J874" s="3"/>
       <c r="K874" s="3"/>
     </row>
@@ -12598,7 +12605,6 @@
       <c r="F879" s="3"/>
       <c r="G879" s="3"/>
       <c r="H879" s="3"/>
-      <c r="I879" s="3"/>
       <c r="J879" s="3"/>
       <c r="K879" s="3"/>
     </row>
@@ -12611,6 +12617,7 @@
       <c r="F880" s="3"/>
       <c r="G880" s="3"/>
       <c r="H880" s="3"/>
+      <c r="I880" s="3"/>
       <c r="J880" s="3"/>
       <c r="K880" s="3"/>
     </row>
@@ -12649,7 +12656,6 @@
       <c r="F883" s="3"/>
       <c r="G883" s="3"/>
       <c r="H883" s="3"/>
-      <c r="I883" s="3"/>
       <c r="J883" s="3"/>
       <c r="K883" s="3"/>
     </row>
@@ -12662,6 +12668,7 @@
       <c r="F884" s="3"/>
       <c r="G884" s="3"/>
       <c r="H884" s="3"/>
+      <c r="I884" s="3"/>
       <c r="J884" s="3"/>
       <c r="K884" s="3"/>
     </row>
@@ -12713,7 +12720,6 @@
       <c r="F888" s="3"/>
       <c r="G888" s="3"/>
       <c r="H888" s="3"/>
-      <c r="I888" s="3"/>
       <c r="J888" s="3"/>
       <c r="K888" s="3"/>
     </row>
@@ -12762,6 +12768,7 @@
       <c r="F892" s="3"/>
       <c r="G892" s="3"/>
       <c r="H892" s="3"/>
+      <c r="I892" s="3"/>
       <c r="J892" s="3"/>
       <c r="K892" s="3"/>
     </row>
@@ -12787,7 +12794,6 @@
       <c r="F894" s="3"/>
       <c r="G894" s="3"/>
       <c r="H894" s="3"/>
-      <c r="I894" s="3"/>
       <c r="J894" s="3"/>
       <c r="K894" s="3"/>
     </row>
@@ -12800,6 +12806,7 @@
       <c r="F895" s="3"/>
       <c r="G895" s="3"/>
       <c r="H895" s="3"/>
+      <c r="I895" s="3"/>
       <c r="J895" s="3"/>
       <c r="K895" s="3"/>
     </row>
@@ -12812,7 +12819,6 @@
       <c r="F896" s="3"/>
       <c r="G896" s="3"/>
       <c r="H896" s="3"/>
-      <c r="I896" s="3"/>
       <c r="J896" s="3"/>
       <c r="K896" s="3"/>
     </row>
@@ -12825,6 +12831,7 @@
       <c r="F897" s="3"/>
       <c r="G897" s="3"/>
       <c r="H897" s="3"/>
+      <c r="I897" s="3"/>
       <c r="J897" s="3"/>
       <c r="K897" s="3"/>
     </row>
@@ -12876,7 +12883,6 @@
       <c r="F901" s="3"/>
       <c r="G901" s="3"/>
       <c r="H901" s="3"/>
-      <c r="I901" s="3"/>
       <c r="J901" s="3"/>
       <c r="K901" s="3"/>
     </row>
@@ -12901,6 +12907,7 @@
       <c r="F903" s="3"/>
       <c r="G903" s="3"/>
       <c r="H903" s="3"/>
+      <c r="I903" s="3"/>
       <c r="J903" s="3"/>
       <c r="K903" s="3"/>
     </row>
@@ -12926,7 +12933,6 @@
       <c r="F905" s="3"/>
       <c r="G905" s="3"/>
       <c r="H905" s="3"/>
-      <c r="I905" s="3"/>
       <c r="J905" s="3"/>
       <c r="K905" s="3"/>
     </row>
@@ -12939,6 +12945,7 @@
       <c r="F906" s="3"/>
       <c r="G906" s="3"/>
       <c r="H906" s="3"/>
+      <c r="I906" s="3"/>
       <c r="J906" s="3"/>
       <c r="K906" s="3"/>
     </row>
@@ -12964,7 +12971,6 @@
       <c r="F908" s="3"/>
       <c r="G908" s="3"/>
       <c r="H908" s="3"/>
-      <c r="I908" s="3"/>
       <c r="J908" s="3"/>
       <c r="K908" s="3"/>
     </row>
@@ -12977,6 +12983,7 @@
       <c r="F909" s="3"/>
       <c r="G909" s="3"/>
       <c r="H909" s="3"/>
+      <c r="I909" s="3"/>
       <c r="J909" s="3"/>
       <c r="K909" s="3"/>
     </row>
@@ -13028,7 +13035,6 @@
       <c r="F913" s="3"/>
       <c r="G913" s="3"/>
       <c r="H913" s="3"/>
-      <c r="I913" s="3"/>
       <c r="J913" s="3"/>
       <c r="K913" s="3"/>
     </row>
@@ -13041,6 +13047,7 @@
       <c r="F914" s="3"/>
       <c r="G914" s="3"/>
       <c r="H914" s="3"/>
+      <c r="I914" s="3"/>
       <c r="J914" s="3"/>
       <c r="K914" s="3"/>
     </row>
@@ -13053,7 +13060,6 @@
       <c r="F915" s="3"/>
       <c r="G915" s="3"/>
       <c r="H915" s="3"/>
-      <c r="I915" s="3"/>
       <c r="J915" s="3"/>
       <c r="K915" s="3"/>
     </row>
@@ -13066,6 +13072,7 @@
       <c r="F916" s="3"/>
       <c r="G916" s="3"/>
       <c r="H916" s="3"/>
+      <c r="I916" s="3"/>
       <c r="J916" s="3"/>
       <c r="K916" s="3"/>
     </row>
@@ -13078,7 +13085,6 @@
       <c r="F917" s="3"/>
       <c r="G917" s="3"/>
       <c r="H917" s="3"/>
-      <c r="I917" s="3"/>
       <c r="J917" s="3"/>
       <c r="K917" s="3"/>
     </row>
@@ -13091,6 +13097,7 @@
       <c r="F918" s="3"/>
       <c r="G918" s="3"/>
       <c r="H918" s="3"/>
+      <c r="I918" s="3"/>
       <c r="J918" s="3"/>
       <c r="K918" s="3"/>
     </row>
@@ -13116,7 +13123,6 @@
       <c r="F920" s="3"/>
       <c r="G920" s="3"/>
       <c r="H920" s="3"/>
-      <c r="I920" s="3"/>
       <c r="J920" s="3"/>
       <c r="K920" s="3"/>
     </row>
@@ -13129,6 +13135,7 @@
       <c r="F921" s="3"/>
       <c r="G921" s="3"/>
       <c r="H921" s="3"/>
+      <c r="I921" s="3"/>
       <c r="J921" s="3"/>
       <c r="K921" s="3"/>
     </row>
@@ -13206,7 +13213,6 @@
       <c r="F927" s="3"/>
       <c r="G927" s="3"/>
       <c r="H927" s="3"/>
-      <c r="I927" s="3"/>
       <c r="J927" s="3"/>
       <c r="K927" s="3"/>
     </row>
@@ -13219,6 +13225,7 @@
       <c r="F928" s="3"/>
       <c r="G928" s="3"/>
       <c r="H928" s="3"/>
+      <c r="I928" s="3"/>
       <c r="J928" s="3"/>
       <c r="K928" s="3"/>
     </row>
@@ -13231,7 +13238,6 @@
       <c r="F929" s="3"/>
       <c r="G929" s="3"/>
       <c r="H929" s="3"/>
-      <c r="I929" s="3"/>
       <c r="J929" s="3"/>
       <c r="K929" s="3"/>
     </row>
@@ -13244,6 +13250,7 @@
       <c r="F930" s="3"/>
       <c r="G930" s="3"/>
       <c r="H930" s="3"/>
+      <c r="I930" s="3"/>
       <c r="J930" s="3"/>
       <c r="K930" s="3"/>
     </row>
@@ -13321,7 +13328,6 @@
       <c r="F936" s="3"/>
       <c r="G936" s="3"/>
       <c r="H936" s="3"/>
-      <c r="I936" s="3"/>
       <c r="J936" s="3"/>
       <c r="K936" s="3"/>
     </row>
@@ -13334,6 +13340,7 @@
       <c r="F937" s="3"/>
       <c r="G937" s="3"/>
       <c r="H937" s="3"/>
+      <c r="I937" s="3"/>
       <c r="J937" s="3"/>
       <c r="K937" s="3"/>
     </row>
@@ -13372,7 +13379,6 @@
       <c r="F940" s="3"/>
       <c r="G940" s="3"/>
       <c r="H940" s="3"/>
-      <c r="I940" s="3"/>
       <c r="J940" s="3"/>
       <c r="K940" s="3"/>
     </row>
@@ -13385,6 +13391,7 @@
       <c r="F941" s="3"/>
       <c r="G941" s="3"/>
       <c r="H941" s="3"/>
+      <c r="I941" s="3"/>
       <c r="J941" s="3"/>
       <c r="K941" s="3"/>
     </row>
@@ -13423,7 +13430,6 @@
       <c r="F944" s="3"/>
       <c r="G944" s="3"/>
       <c r="H944" s="3"/>
-      <c r="I944" s="3"/>
       <c r="J944" s="3"/>
       <c r="K944" s="3"/>
     </row>
@@ -13448,6 +13454,7 @@
       <c r="F946" s="3"/>
       <c r="G946" s="3"/>
       <c r="H946" s="3"/>
+      <c r="I946" s="3"/>
       <c r="J946" s="3"/>
       <c r="K946" s="3"/>
     </row>
@@ -13512,7 +13519,6 @@
       <c r="F951" s="3"/>
       <c r="G951" s="3"/>
       <c r="H951" s="3"/>
-      <c r="I951" s="3"/>
       <c r="J951" s="3"/>
       <c r="K951" s="3"/>
     </row>
@@ -13525,6 +13531,7 @@
       <c r="F952" s="3"/>
       <c r="G952" s="3"/>
       <c r="H952" s="3"/>
+      <c r="I952" s="3"/>
       <c r="J952" s="3"/>
       <c r="K952" s="3"/>
     </row>
@@ -13537,7 +13544,6 @@
       <c r="F953" s="3"/>
       <c r="G953" s="3"/>
       <c r="H953" s="3"/>
-      <c r="I953" s="3"/>
       <c r="J953" s="3"/>
       <c r="K953" s="3"/>
     </row>
@@ -13562,6 +13568,7 @@
       <c r="F955" s="3"/>
       <c r="G955" s="3"/>
       <c r="H955" s="3"/>
+      <c r="I955" s="3"/>
       <c r="J955" s="3"/>
       <c r="K955" s="3"/>
     </row>
@@ -13625,8 +13632,6 @@
       <c r="E960" s="3"/>
       <c r="F960" s="3"/>
       <c r="G960" s="3"/>
-      <c r="H960" s="3"/>
-      <c r="I960" s="3"/>
       <c r="J960" s="3"/>
       <c r="K960" s="3"/>
     </row>
@@ -13638,6 +13643,7 @@
       <c r="E961" s="3"/>
       <c r="F961" s="3"/>
       <c r="G961" s="3"/>
+      <c r="H961" s="3"/>
       <c r="J961" s="3"/>
       <c r="K961" s="3"/>
     </row>
@@ -13650,6 +13656,7 @@
       <c r="F962" s="3"/>
       <c r="G962" s="3"/>
       <c r="H962" s="3"/>
+      <c r="I962" s="3"/>
       <c r="J962" s="3"/>
       <c r="K962" s="3"/>
     </row>
@@ -13675,7 +13682,6 @@
       <c r="F964" s="3"/>
       <c r="G964" s="3"/>
       <c r="H964" s="3"/>
-      <c r="I964" s="3"/>
       <c r="J964" s="3"/>
       <c r="K964" s="3"/>
     </row>
@@ -13724,6 +13730,7 @@
       <c r="F968" s="3"/>
       <c r="G968" s="3"/>
       <c r="H968" s="3"/>
+      <c r="I968" s="3"/>
       <c r="J968" s="3"/>
       <c r="K968" s="3"/>
     </row>
@@ -13775,7 +13782,6 @@
       <c r="F972" s="3"/>
       <c r="G972" s="3"/>
       <c r="H972" s="3"/>
-      <c r="I972" s="3"/>
       <c r="J972" s="3"/>
       <c r="K972" s="3"/>
     </row>
@@ -13788,6 +13794,7 @@
       <c r="F973" s="3"/>
       <c r="G973" s="3"/>
       <c r="H973" s="3"/>
+      <c r="I973" s="3"/>
       <c r="J973" s="3"/>
       <c r="K973" s="3"/>
     </row>
@@ -13800,7 +13807,6 @@
       <c r="F974" s="3"/>
       <c r="G974" s="3"/>
       <c r="H974" s="3"/>
-      <c r="I974" s="3"/>
       <c r="J974" s="3"/>
       <c r="K974" s="3"/>
     </row>
@@ -13813,6 +13819,7 @@
       <c r="F975" s="3"/>
       <c r="G975" s="3"/>
       <c r="H975" s="3"/>
+      <c r="I975" s="3"/>
       <c r="J975" s="3"/>
       <c r="K975" s="3"/>
     </row>
@@ -13825,7 +13832,6 @@
       <c r="F976" s="3"/>
       <c r="G976" s="3"/>
       <c r="H976" s="3"/>
-      <c r="I976" s="3"/>
       <c r="J976" s="3"/>
       <c r="K976" s="3"/>
     </row>
@@ -13838,6 +13844,7 @@
       <c r="F977" s="3"/>
       <c r="G977" s="3"/>
       <c r="H977" s="3"/>
+      <c r="I977" s="3"/>
       <c r="J977" s="3"/>
       <c r="K977" s="3"/>
     </row>
@@ -13876,7 +13883,6 @@
       <c r="F980" s="3"/>
       <c r="G980" s="3"/>
       <c r="H980" s="3"/>
-      <c r="I980" s="3"/>
       <c r="J980" s="3"/>
       <c r="K980" s="3"/>
     </row>
@@ -13901,6 +13907,7 @@
       <c r="F982" s="3"/>
       <c r="G982" s="3"/>
       <c r="H982" s="3"/>
+      <c r="I982" s="3"/>
       <c r="J982" s="3"/>
       <c r="K982" s="3"/>
     </row>
@@ -13978,7 +13985,6 @@
       <c r="F988" s="3"/>
       <c r="G988" s="3"/>
       <c r="H988" s="3"/>
-      <c r="I988" s="3"/>
       <c r="J988" s="3"/>
       <c r="K988" s="3"/>
     </row>
@@ -13991,6 +13997,7 @@
       <c r="F989" s="3"/>
       <c r="G989" s="3"/>
       <c r="H989" s="3"/>
+      <c r="I989" s="3"/>
       <c r="J989" s="3"/>
       <c r="K989" s="3"/>
     </row>
@@ -14003,7 +14010,6 @@
       <c r="F990" s="3"/>
       <c r="G990" s="3"/>
       <c r="H990" s="3"/>
-      <c r="I990" s="3"/>
       <c r="J990" s="3"/>
       <c r="K990" s="3"/>
     </row>
@@ -14028,6 +14034,7 @@
       <c r="F992" s="3"/>
       <c r="G992" s="3"/>
       <c r="H992" s="3"/>
+      <c r="I992" s="3"/>
       <c r="J992" s="3"/>
       <c r="K992" s="3"/>
     </row>
@@ -14053,7 +14060,6 @@
       <c r="F994" s="3"/>
       <c r="G994" s="3"/>
       <c r="H994" s="3"/>
-      <c r="I994" s="3"/>
       <c r="J994" s="3"/>
       <c r="K994" s="3"/>
     </row>
@@ -14066,6 +14072,7 @@
       <c r="F995" s="3"/>
       <c r="G995" s="3"/>
       <c r="H995" s="3"/>
+      <c r="I995" s="3"/>
       <c r="J995" s="3"/>
       <c r="K995" s="3"/>
     </row>
@@ -14078,7 +14085,6 @@
       <c r="F996" s="3"/>
       <c r="G996" s="3"/>
       <c r="H996" s="3"/>
-      <c r="I996" s="3"/>
       <c r="J996" s="3"/>
       <c r="K996" s="3"/>
     </row>
@@ -14103,6 +14109,7 @@
       <c r="F998" s="3"/>
       <c r="G998" s="3"/>
       <c r="H998" s="3"/>
+      <c r="I998" s="3"/>
       <c r="J998" s="3"/>
       <c r="K998" s="3"/>
     </row>
@@ -14245,7 +14252,6 @@
       <c r="F1009" s="3"/>
       <c r="G1009" s="3"/>
       <c r="H1009" s="3"/>
-      <c r="I1009" s="3"/>
       <c r="J1009" s="3"/>
       <c r="K1009" s="3"/>
     </row>
@@ -14258,6 +14264,7 @@
       <c r="F1010" s="3"/>
       <c r="G1010" s="3"/>
       <c r="H1010" s="3"/>
+      <c r="I1010" s="3"/>
       <c r="J1010" s="3"/>
       <c r="K1010" s="3"/>
     </row>
@@ -14283,7 +14290,6 @@
       <c r="F1012" s="3"/>
       <c r="G1012" s="3"/>
       <c r="H1012" s="3"/>
-      <c r="I1012" s="3"/>
       <c r="J1012" s="3"/>
       <c r="K1012" s="3"/>
     </row>
@@ -14296,6 +14302,7 @@
       <c r="F1013" s="3"/>
       <c r="G1013" s="3"/>
       <c r="H1013" s="3"/>
+      <c r="I1013" s="3"/>
       <c r="J1013" s="3"/>
       <c r="K1013" s="3"/>
     </row>
@@ -14308,7 +14315,6 @@
       <c r="F1014" s="3"/>
       <c r="G1014" s="3"/>
       <c r="H1014" s="3"/>
-      <c r="I1014" s="3"/>
       <c r="J1014" s="3"/>
       <c r="K1014" s="3"/>
     </row>
@@ -14321,6 +14327,7 @@
       <c r="F1015" s="3"/>
       <c r="G1015" s="3"/>
       <c r="H1015" s="3"/>
+      <c r="I1015" s="3"/>
       <c r="J1015" s="3"/>
       <c r="K1015" s="3"/>
     </row>
@@ -14333,7 +14340,6 @@
       <c r="F1016" s="3"/>
       <c r="G1016" s="3"/>
       <c r="H1016" s="3"/>
-      <c r="I1016" s="3"/>
       <c r="J1016" s="3"/>
       <c r="K1016" s="3"/>
     </row>
@@ -14346,6 +14352,7 @@
       <c r="F1017" s="3"/>
       <c r="G1017" s="3"/>
       <c r="H1017" s="3"/>
+      <c r="I1017" s="3"/>
       <c r="J1017" s="3"/>
       <c r="K1017" s="3"/>
     </row>
@@ -14358,7 +14365,6 @@
       <c r="F1018" s="3"/>
       <c r="G1018" s="3"/>
       <c r="H1018" s="3"/>
-      <c r="I1018" s="3"/>
       <c r="J1018" s="3"/>
       <c r="K1018" s="3"/>
     </row>
@@ -14371,6 +14377,7 @@
       <c r="F1019" s="3"/>
       <c r="G1019" s="3"/>
       <c r="H1019" s="3"/>
+      <c r="I1019" s="3"/>
       <c r="J1019" s="3"/>
       <c r="K1019" s="3"/>
     </row>
@@ -14409,7 +14416,6 @@
       <c r="F1022" s="3"/>
       <c r="G1022" s="3"/>
       <c r="H1022" s="3"/>
-      <c r="I1022" s="3"/>
       <c r="J1022" s="3"/>
       <c r="K1022" s="3"/>
     </row>
@@ -14422,6 +14428,7 @@
       <c r="F1023" s="3"/>
       <c r="G1023" s="3"/>
       <c r="H1023" s="3"/>
+      <c r="I1023" s="3"/>
       <c r="J1023" s="3"/>
       <c r="K1023" s="3"/>
     </row>
@@ -14447,7 +14454,6 @@
       <c r="F1025" s="3"/>
       <c r="G1025" s="3"/>
       <c r="H1025" s="3"/>
-      <c r="I1025" s="3"/>
       <c r="J1025" s="3"/>
       <c r="K1025" s="3"/>
     </row>
@@ -14460,6 +14466,7 @@
       <c r="F1026" s="3"/>
       <c r="G1026" s="3"/>
       <c r="H1026" s="3"/>
+      <c r="I1026" s="3"/>
       <c r="J1026" s="3"/>
       <c r="K1026" s="3"/>
     </row>
@@ -14550,7 +14557,6 @@
       <c r="F1033" s="3"/>
       <c r="G1033" s="3"/>
       <c r="H1033" s="3"/>
-      <c r="I1033" s="3"/>
       <c r="J1033" s="3"/>
       <c r="K1033" s="3"/>
     </row>
@@ -14575,6 +14581,7 @@
       <c r="F1035" s="3"/>
       <c r="G1035" s="3"/>
       <c r="H1035" s="3"/>
+      <c r="I1035" s="3"/>
       <c r="J1035" s="3"/>
       <c r="K1035" s="3"/>
     </row>
@@ -14587,7 +14594,6 @@
       <c r="F1036" s="3"/>
       <c r="G1036" s="3"/>
       <c r="H1036" s="3"/>
-      <c r="I1036" s="3"/>
       <c r="J1036" s="3"/>
       <c r="K1036" s="3"/>
     </row>
@@ -14600,21 +14606,9 @@
       <c r="F1037" s="3"/>
       <c r="G1037" s="3"/>
       <c r="H1037" s="3"/>
+      <c r="I1037" s="3"/>
       <c r="J1037" s="3"/>
       <c r="K1037" s="3"/>
-    </row>
-    <row r="1038" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1038" s="3"/>
-      <c r="B1038" s="3"/>
-      <c r="C1038" s="3"/>
-      <c r="D1038" s="3"/>
-      <c r="E1038" s="3"/>
-      <c r="F1038" s="3"/>
-      <c r="G1038" s="3"/>
-      <c r="H1038" s="3"/>
-      <c r="I1038" s="3"/>
-      <c r="J1038" s="3"/>
-      <c r="K1038" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>